<commit_message>
Update How to work with papers.docx, Ideas and goals.docx, and 11 more files...
</commit_message>
<xml_diff>
--- a/papers/references.xlsx
+++ b/papers/references.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ansk\github\Master-s-thesis\papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7D5495-8687-496A-9F0A-A2B8AFD43954}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A9A656B-D404-4395-B474-B01BDE9210E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Model-driven engineering" sheetId="1" r:id="rId1"/>
+    <sheet name="Software factories" sheetId="2" r:id="rId2"/>
+    <sheet name="Models and metamodels" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Citation</t>
   </si>
@@ -36,13 +38,65 @@
     <t>Why important</t>
   </si>
   <si>
-    <t>Where placed</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
     <t>Key notes</t>
+  </si>
+  <si>
+    <t>"@article{article,
+author = {Hailpern, Brent and Tarr, P.},
+year = {2006},
+month = {02},
+pages = {451 - 461},
+title = {Model-driven development: The good, the bad, and the ugly},
+volume = {45},
+journal = {IBM Systems Journal},
+doi = {10.1147/sj.453.0451}
+}"</t>
+  </si>
+  <si>
+    <t>Model-driven development: The good, the bad, and the ugly</t>
+  </si>
+  <si>
+    <t>"@inproceedings{sen2007partial,
+  title={Partial model completion in model driven engineering using constraint logic programming},
+  author={Sen, Sagar and Baudry, Benoit and Precup, Doina},
+  booktitle={17th International Conference on Applications of Declarative Programming and Knowledge Management (INAP 2007) and 21st Workshop on (Constraint)},
+  pages={59},
+  year={2007}
+}"</t>
+  </si>
+  <si>
+    <t>Partial model completion in model driven engineering using constraint logic programming</t>
+  </si>
+  <si>
+    <t>"@article{wahler2007model,
+  title={Model-driven constraint engineering},
+  author={Wahler, Michael and Koehler, Jana and Brucker, Achim D},
+  journal={Electronic Communications of the EASST},
+  volume={5},
+  year={2007}
+}"</t>
+  </si>
+  <si>
+    <t>Model-driven constraint engineering</t>
+  </si>
+  <si>
+    <t>Model-driven development: a metamodeling foundation</t>
+  </si>
+  <si>
+    <t>"@article{1231149,  author={Atkinson, C. and Kuhne, T.},  journal={IEEE Software},   title={Model-driven development: a metamodeling foundation},   year={2003},  volume={20},  number={5},  pages={36-41},  doi={10.1109/MS.2003.1231149}}"</t>
+  </si>
+  <si>
+    <t>"@inproceedings{bezivin2005model,
+  title={Model driven engineering: An emerging technical space},
+  author={B{\'e}zivin, Jean},
+  booktitle={International Summer School on Generative and Transformational Techniques in Software Engineering},
+  pages={36--64},
+  year={2005},
+  organization={Springer}
+}"</t>
+  </si>
+  <si>
+    <t>Model Driven Engineering: An Emerging Technical Space</t>
   </si>
 </sst>
 </file>
@@ -66,7 +120,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -74,17 +128,234 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="9">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -98,15 +369,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8285077E-5915-4057-BA77-1D27902F310A}" name="Table1" displayName="Table1" ref="A1:F15" totalsRowShown="0">
-  <autoFilter ref="A1:F15" xr:uid="{BA718EE1-49D7-4650-B037-0771614423BF}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{FF3B8A2A-F932-41FA-95FE-F39F73C1F2C4}" name="Citation"/>
-    <tableColumn id="2" xr3:uid="{9B6745B4-27F0-426A-8DDC-565EB29CD89F}" name="Paper"/>
-    <tableColumn id="3" xr3:uid="{740F9031-EF03-4B61-BD05-ED6CA620EB43}" name="Where placed"/>
-    <tableColumn id="4" xr3:uid="{E2A44B50-6AB1-4D21-B405-3EA821BDC969}" name="Category"/>
-    <tableColumn id="5" xr3:uid="{07897410-23B2-4D10-BE84-96D70F98FBC6}" name="Why important"/>
-    <tableColumn id="6" xr3:uid="{A1146B1C-F33C-432E-90B6-E265AC99A77B}" name="Key notes"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8285077E-5915-4057-BA77-1D27902F310A}" name="Table1" displayName="Table1" ref="A1:D6" totalsRowShown="0" headerRowDxfId="5" dataDxfId="0" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
+  <autoFilter ref="A1:D6" xr:uid="{BA718EE1-49D7-4650-B037-0771614423BF}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{FF3B8A2A-F932-41FA-95FE-F39F73C1F2C4}" name="Citation" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{9B6745B4-27F0-426A-8DDC-565EB29CD89F}" name="Paper" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{07897410-23B2-4D10-BE84-96D70F98FBC6}" name="Why important" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{A1146B1C-F33C-432E-90B6-E265AC99A77B}" name="Key notes" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -375,45 +644,119 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="10.44140625" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" customWidth="1"/>
-    <col min="4" max="4" width="15.21875" customWidth="1"/>
+    <col min="1" max="1" width="23.21875" customWidth="1"/>
+    <col min="2" max="2" width="26.5546875" customWidth="1"/>
+    <col min="3" max="3" width="30" customWidth="1"/>
+    <col min="4" max="4" width="121.21875" customWidth="1"/>
     <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6"/>
+    </row>
+    <row r="3" spans="1:4" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="1:4" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="6"/>
+    </row>
+    <row r="5" spans="1:4" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="1:4" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CF1A488-2851-4C66-A331-30E6C95E0D1D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3F4F4E1-D1E9-4F42-9C7C-394B46E3D0E8}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update How to work with papers.docx, MA Plan.docx, and 2 more files...
</commit_message>
<xml_diff>
--- a/papers/references.xlsx
+++ b/papers/references.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ansk\github\Master-s-thesis\papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A9A656B-D404-4395-B474-B01BDE9210E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3028BF-3789-49D3-AA6A-E76BC886A787}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,18 +27,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Citation</t>
   </si>
   <si>
     <t>Paper</t>
-  </si>
-  <si>
-    <t>Why important</t>
-  </si>
-  <si>
-    <t>Key notes</t>
   </si>
   <si>
     <t>"@article{article,
@@ -97,6 +91,68 @@
   </si>
   <si>
     <t>Model Driven Engineering: An Emerging Technical Space</t>
+  </si>
+  <si>
+    <t>Goals</t>
+  </si>
+  <si>
+    <t>Used methods</t>
+  </si>
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>Why important (one sentence)</t>
+  </si>
+  <si>
+    <t>Give an overview of what the MDE is, its origination roots, and its current state; specifically how it can be used in modern software systems</t>
+  </si>
+  <si>
+    <t>Definitions of model, mde and its key componetns</t>
+  </si>
+  <si>
+    <t>Course defitions of a model, mde, model transformation</t>
+  </si>
+  <si>
+    <t>"@article{bezivin2004search,
+  title={In search of a basic principle for model driven engineering},
+  author={B{\'e}zivin, Jean},
+  journal={Novatica Journal, Special Issue},
+  volume={5},
+  number={2},
+  pages={21--24},
+  year={2004},
+  publisher={Citeseer}
+}"</t>
+  </si>
+  <si>
+    <t>In search of a basic principle for model driven engineering</t>
+  </si>
+  <si>
+    <t>find fundamental ideas of MDE</t>
+  </si>
+  <si>
+    <t>Similar to the term "everything is an object" define a statement "everything is a model" in the scope of MDA to look for the essential trates of MDE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model is a graph-oriented structure to present a certain domain in its simplified but coherent representation which adheres to another graph structure named metamodel; MDE is an approach that relies on three components that are closely related to each other: automation, DSL, and commonly-agreed standards; MDE is as a technique to create software products by considering models and their elements as the most important construction blocks; </t>
+  </si>
+  <si>
+    <t>What is MDA</t>
+  </si>
+  <si>
+    <t>MDA is regarded as a practical implementation of MDE that was created with the use of OMG standards;
+a Switch of the paradigm to viewing not an object as a central element of the systems but model and its elements. This allows us to consider models not just as a form of representing documentation but as a complete space to drive software product lines; 
+After the introduction of MDA by OMG Group, the transition from code-based to model-based software happened. This, in turn, induced the appearance of many languages used to specify a certain domain. The variety of different meta-languages urged the need to create a unified framework that all meta-languages could conform to and, thus, to make them interchangeable. That is how emerged MOF - a unified modeling language for all meta-models;</t>
+  </si>
+  <si>
+    <t>Remove the good ideas behind MDE, its limitation and the bad part of MDE</t>
+  </si>
+  <si>
+    <t>Analysis of MDE and its limitations through analysis</t>
+  </si>
+  <si>
+    <t>A desire to reduce the time to market for software systems, their continuously growing complexity, and ongoing demand for higher software quality was an incentive to look for some automation tools. As a result, the concept of MDE appeared; A straightforward but not the smartest approach to implement some system is to have some log with requirements and present architecture as some figures with available interfaces. Based on it, developers tend directly writing source code. The list of bugs is kept in some issue-tracking products. Taking into account that by such an approach the requirements are not mapped to architecture and source code, then it becomes extremely difficult to reflect this match during the implementation stage. Gradually it might become even worse as soon as the code base begins to age and produce even more bugs. The solution to overcome those problems seems obvious. If one has an overarching single data source that would link to each other all the stages of software development, it would help keep all aspects of development interconnected to each other;</t>
   </si>
 </sst>
 </file>
@@ -120,7 +176,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -204,11 +260,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -234,13 +301,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="11">
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -307,6 +407,39 @@
       </border>
     </dxf>
     <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -323,36 +456,6 @@
         <horizontal style="thin">
           <color indexed="64"/>
         </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
   </dxfs>
@@ -369,13 +472,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8285077E-5915-4057-BA77-1D27902F310A}" name="Table1" displayName="Table1" ref="A1:D6" totalsRowShown="0" headerRowDxfId="5" dataDxfId="0" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
-  <autoFilter ref="A1:D6" xr:uid="{BA718EE1-49D7-4650-B037-0771614423BF}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{FF3B8A2A-F932-41FA-95FE-F39F73C1F2C4}" name="Citation" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{9B6745B4-27F0-426A-8DDC-565EB29CD89F}" name="Paper" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{07897410-23B2-4D10-BE84-96D70F98FBC6}" name="Why important" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{A1146B1C-F33C-432E-90B6-E265AC99A77B}" name="Key notes" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8285077E-5915-4057-BA77-1D27902F310A}" name="Table1" displayName="Table1" ref="A1:F7" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+  <autoFilter ref="A1:F7" xr:uid="{BA718EE1-49D7-4650-B037-0771614423BF}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{FF3B8A2A-F932-41FA-95FE-F39F73C1F2C4}" name="Citation" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{9B6745B4-27F0-426A-8DDC-565EB29CD89F}" name="Paper" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{07897410-23B2-4D10-BE84-96D70F98FBC6}" name="Goals" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{A1146B1C-F33C-432E-90B6-E265AC99A77B}" name="Used methods" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{04662BCC-AEE1-4C61-887F-F2AF7BAE3722}" name="Results" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{0DF0A271-EB9F-4F3F-959F-4DECC9AAB759}" name="Why important (one sentence)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -644,10 +749,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -655,12 +760,12 @@
     <col min="1" max="1" width="23.21875" customWidth="1"/>
     <col min="2" max="2" width="26.5546875" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="121.21875" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5546875" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="64.44140625" customWidth="1"/>
+    <col min="6" max="6" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -668,61 +773,111 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
+      <c r="C2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="9"/>
     </row>
-    <row r="2" spans="1:4" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+    <row r="3" spans="1:6" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B3" s="5" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6"/>
-    </row>
-    <row r="3" spans="1:4" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>7</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="8"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:4" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:4" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:4" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="6"/>
+        <v>11</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
MDE/MDA chapter is ready
</commit_message>
<xml_diff>
--- a/papers/references.xlsx
+++ b/papers/references.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ansk\github\Master-s-thesis\papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3028BF-3789-49D3-AA6A-E76BC886A787}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B869444-CBD9-41C6-9E4E-253DDE15FB9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>Citation</t>
   </si>
@@ -135,32 +135,85 @@
     <t>Similar to the term "everything is an object" define a statement "everything is a model" in the scope of MDA to look for the essential trates of MDE</t>
   </si>
   <si>
-    <t xml:space="preserve">Model is a graph-oriented structure to present a certain domain in its simplified but coherent representation which adheres to another graph structure named metamodel; MDE is an approach that relies on three components that are closely related to each other: automation, DSL, and commonly-agreed standards; MDE is as a technique to create software products by considering models and their elements as the most important construction blocks; </t>
-  </si>
-  <si>
     <t>What is MDA</t>
   </si>
   <si>
-    <t>MDA is regarded as a practical implementation of MDE that was created with the use of OMG standards;
-a Switch of the paradigm to viewing not an object as a central element of the systems but model and its elements. This allows us to consider models not just as a form of representing documentation but as a complete space to drive software product lines; 
-After the introduction of MDA by OMG Group, the transition from code-based to model-based software happened. This, in turn, induced the appearance of many languages used to specify a certain domain. The variety of different meta-languages urged the need to create a unified framework that all meta-languages could conform to and, thus, to make them interchangeable. That is how emerged MOF - a unified modeling language for all meta-models;</t>
-  </si>
-  <si>
-    <t>Remove the good ideas behind MDE, its limitation and the bad part of MDE</t>
-  </si>
-  <si>
     <t>Analysis of MDE and its limitations through analysis</t>
   </si>
   <si>
-    <t>A desire to reduce the time to market for software systems, their continuously growing complexity, and ongoing demand for higher software quality was an incentive to look for some automation tools. As a result, the concept of MDE appeared; A straightforward but not the smartest approach to implement some system is to have some log with requirements and present architecture as some figures with available interfaces. Based on it, developers tend directly writing source code. The list of bugs is kept in some issue-tracking products. Taking into account that by such an approach the requirements are not mapped to architecture and source code, then it becomes extremely difficult to reflect this match during the implementation stage. Gradually it might become even worse as soon as the code base begins to age and produce even more bugs. The solution to overcome those problems seems obvious. If one has an overarching single data source that would link to each other all the stages of software development, it would help keep all aspects of development interconnected to each other;</t>
+    <t>MDA key features and limitaions</t>
+  </si>
+  <si>
+    <t>Define requirements of MDD and provide a universal MDD infrastructure</t>
+  </si>
+  <si>
+    <t>Role of metamodelling in MDD</t>
+  </si>
+  <si>
+    <t>Reveal the good ideas behind MDE, its limitation and the bad part of MDE</t>
+  </si>
+  <si>
+    <t>Constraint met-level of MDE -&gt; to make them precise</t>
+  </si>
+  <si>
+    <t>Developed a tool</t>
+  </si>
+  <si>
+    <t>It's rather related to my related work and to some ideas for my implementation</t>
+  </si>
+  <si>
+    <t>Define constrain types and templates for them</t>
+  </si>
+  <si>
+    <t>Model completion</t>
+  </si>
+  <si>
+    <t>Design a tool for model completion in MDE using constraint programming</t>
+  </si>
+  <si>
+    <t>Constraint logic program</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The concept of MDE was first presented and coined by {?} in {?} as a promising solution to overcome new challenges of developing industrial software systems. The continuous increase in software complexity, the ongoing demand for higher product quality, and the requirement to reduce time to market are the main milestones that identified the need for automation tools while implementing complex software systems.
+An oversimplified process to design software with no success guarantees consists of the following steps. First, requirements are captured in a textual form. Secondly, the overall system architecture is presented as a list of figures that depict inbound and outbound interfaces. Equipped with that, developers tend to write source code. However, the fundamental problem with that approach is that all stages of the software development life cycle have no inter-relation. In other words, the whole process lacks a uniform domain of knowledge. For instance, what are the chances that a revealed bug during the maintenance stage is going to be fixed with no other harmful side-effects to the system if no mapping exists from the code base to architecture and requirements? The answer is that it is unlikely to happen. A feasible solution to this issue is to have a single overarching metamodel that would link all the aspects of a software system and would allow transforming one model view to another one with no negative consequences.
+One of the essential concepts of MDE is to both simplify and standardize all levels of the software life cycle to make automation possible.
+One of the pioneers in applying broad MDE concepts was the Object Management Group (OMG). The OMG group introduced the MDA to support the process of creating software ranging from system requirements to software implementation. MDA classifies multiple levels of system abstraction. Each abstraction represents a model that contains relevant information. Thus, at a higher level of abstraction, one defines a model with business rules without assumptions about technological space. This type of model is also known as PIM. The next step is to generate a platform-specific model (PSM) that contains implementation blocks in one precise technology. The further usage of PSM should result in concrete source code generation. It should also be noted that one PIM might be used to derive an arbitrary number of PSM models. To prevent a manual transition from a higher abstraction level to a lower one, MDA supports and encourages the use of transformation tools to automate this routine.
+The [author] claims that the MDA concept possesses some weaknesses. Firstly, the MDA imposes an abundance of multiple distinct abstraction views on a system. Secondly, the side effects of round-trip engineering cannot be neglected when a change in one model triggers changes in other models. Even one untracked mistake can bring the whole software into inconsistency. One way to tolerate those consequences is to apply constraints to models and their relationships at their meta-level. One of the following chapters evaluates the notion and necessity of constraints in software products.
+</t>
+  </si>
+  <si>
+    <t>The purpose of metamodels and constraints is to enrich a model graph with structural and behavioral elements of a software system. In MDA, MOF serves as a metamodel. Model constraints are specified by OCL that are often embedded into a graphical UML tool to build models and relationships.</t>
+  </si>
+  <si>
+    <t>An MDE infrastructure should support utilities for model interchange and user mappings from models to other artifacts. To tackle it, the use of meta-levels is highly advantageous because it permits model customization to any domain and the addition of new types of models directly at runtime.
+A classical MDE comprises four levels. Every level except the top one regards as an instance-of relation of a higher level. The ground-level M0 stores concrete data that software must operate on. Hence, this level is considered a user-data level. The next M1 level illustrates models that are instantiated for usage in the M0 level. The next M2 level is a metamodel that contains concepts used in the M1 level. The root of a classical MDD hierarchy is M3 meta-metamodel layer (also called Meta-Object-Facility) that inhabits all available notions for its derived subclasses. By adopting such a four-layer architecture, MDE supports introducing new modeling standards as instances of the M3 level. Such infrastructure permits the exchange of information across MOF-compatible models.</t>
+  </si>
+  <si>
+    <t>A model is a graph-oriented structure to describe a domain in its simplified but coherent representation. Each model must adhere to another graph structure named metamodel.
+MDE is an approach that relies on three components that are closely related to each other: automation, DSL, and commonly-agreed standards.
+Standards are necessary to enable a transparent exchange of information.  Automation is essential to bridge the semantical domain specification to concrete technology implementation. DSLs help couple a problem space with solutions for domain experts.
+MDE is a technique to create software products by considering models and their elements as the most important construction components.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Earlier objects played a central role in creating systems. However, with the introduction of MDA a paradigm switch happened. MDA views models and their elements as an essential part of developing software. It means that models drive software product lines and not just as a means of mere documentation.
+MDA initiated the transition from code-based to model-based software development. It induced the release of many languages used to specify a software domain. The variety of domain-specific languages encouraged the creation of a unified framework that all meta-languages could conform to and, thus, make them interchangeable. That was one of the reasons for designing MOF - a meta-meta language for all meta-models;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -275,7 +328,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -295,16 +348,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -751,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -793,15 +849,17 @@
         <v>3</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" s="9"/>
+        <v>24</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="3" spans="1:6" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
@@ -810,22 +868,38 @@
       <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
+      <c r="C3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
+      <c r="C4" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
@@ -834,10 +908,18 @@
       <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
+      <c r="C5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
@@ -852,14 +934,14 @@
       <c r="D6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="10" t="s">
+      <c r="E6" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>19</v>
       </c>
@@ -873,10 +955,10 @@
         <v>22</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
On the way to writing models and metamodels subchapter
</commit_message>
<xml_diff>
--- a/papers/references.xlsx
+++ b/papers/references.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ansk\github\Master-s-thesis\papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B869444-CBD9-41C6-9E4E-253DDE15FB9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B1B566E-5F2C-47CE-857E-60E18D6E88AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model-driven engineering" sheetId="1" r:id="rId1"/>
-    <sheet name="Software factories" sheetId="2" r:id="rId2"/>
-    <sheet name="Models and metamodels" sheetId="3" r:id="rId3"/>
+    <sheet name="Models and metamodels" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="63">
   <si>
     <t>Citation</t>
   </si>
@@ -198,6 +197,124 @@
     <t xml:space="preserve">
 Earlier objects played a central role in creating systems. However, with the introduction of MDA a paradigm switch happened. MDA views models and their elements as an essential part of developing software. It means that models drive software product lines and not just as a means of mere documentation.
 MDA initiated the transition from code-based to model-based software development. It induced the release of many languages used to specify a software domain. The variety of domain-specific languages encouraged the creation of a unified framework that all meta-languages could conform to and, thus, make them interchangeable. That was one of the reasons for designing MOF - a meta-meta language for all meta-models;</t>
+  </si>
+  <si>
+    <t>"@inproceedings{kurpjuweit2007based,
+  title={based Meta Model Engineering.},
+  author={Kurpjuweit, Stephan and Winter, Robert},
+  booktitle={EMISA},
+  volume={143},
+  pages={2007},
+  year={2007}
+}"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viewpoint-based Meta Model Engineering </t>
+  </si>
+  <si>
+    <t>"@inproceedings{atkinson2002role,
+  title={The role of metamodeling in MDA},
+  author={Atkinson, Colin and K{\"u}hne, Thomas},
+  booktitle={Proc. UML 2002 Workshop on Software Model Engineering},
+  pages={67--70},
+  year={2002},
+  organization={Citeseer}
+}"</t>
+  </si>
+  <si>
+    <t>The role of metamodeling in MDA</t>
+  </si>
+  <si>
+    <t>Define the role of metamodelling in MDA</t>
+  </si>
+  <si>
+    <t>Motivation of metamodeling for MDA and requirements for MDA to be conformed to</t>
+  </si>
+  <si>
+    <t>Managing new requirements for software that is in production might get cumbersome. Given the fact that most software systems must meet high availability requirements, it is necessary to perform ad-hoc updates at runtime without bringing the whole system down. For example, a banking system that serves transactions of millions of clients worldwide must have no unscheduled downtime and as least planned maintenance as possible. [Author] claims that it is hardly feasible to deal with newly added requirements by just using the standard means of object-oriented development. Instead, a solution is to introduce an additional meta-level for adding new domain attributes at runtime;</t>
+  </si>
+  <si>
+    <t>Why standard meta model is not enough to fulfill perfect MDA. Describe point that MDA should conform to.</t>
+  </si>
+  <si>
+    <t>Model driven architecture: principles and practice</t>
+  </si>
+  <si>
+    <t>"@article{brown2004model,
+  title={Model driven architecture: Principles and practice},
+  author={Brown, Alan W},
+  journal={Software and systems modeling},
+  volume={3},
+  number={4},
+  pages={314--327},
+  year={2004},
+  publisher={Springer}
+}"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modeling takes one of the most meaningful niches. All sociologists, physicists, chemics, mathematicians, and many other individuals of different areas of occupations construct models in distinct domains. Of course, in the presence of increasing software complexity and the need to exchange information between domain experts and developers concisely, models also play a crucial role in information systems. (my words);
+Before moving on, it is vital to define a definition of a model. According to Brown (Model driven architecture: principles and practice), a model is an abstraction that allows experts to reason about a system by focusing on relevant properties and neglecting secondary ones;
+Complex software systems nowadays tend to be described by multiple models residing on different abstraction levels. The support for model visualization, semantic definition, and transformation is implied by the metamodel. For example, the notion and definition of UML are captured in its metamodel. The UML metamodel defines the core elements such as class, association, multiplicity, and connections among them. The definition of those elements in a metamodel lets the end-user capture properties of a system via diagrams.
+</t>
+  </si>
+  <si>
+    <t>Definition of a model and metamodel</t>
+  </si>
+  <si>
+    <t>Present new metamodeling approach to reflect requirements of multiple stakeholders and map all them in one metamodel</t>
+  </si>
+  <si>
+    <t>Much talks about models and metamodels</t>
+  </si>
+  <si>
+    <t>Designing a metamodel means defining a set of notions used in a model;
+As mentioned in [author], a model should reflect three essential features. First, it should be mapped to its original and represent it. Second, it must have a subset of relevant properties reflected in its original. Finally, it must have a clear objective;
+Although the purpose domain of models to be applied varies a lot depending on the field, three main groups of models should be highlighted. The first group is for the exchange of information and documentation of artifacts. The next one is for some field analysis and its characterization. The last one is to architect and design a given domain;</t>
+  </si>
+  <si>
+    <t>MODEL-DRIVEN
+SOFTWARE ENGINEERING
+IN PRACTICE</t>
+  </si>
+  <si>
+    <t>It is not possible to define models without a proper tool. The class of modeling languages is used to allow specialists to construct models. According to [author] there are two classes of modeling languages.
+1) General-purpose-modeling languages are tools to describe any domain or specialization. Some of the representatives of this kind of language are JAVA or UML.
+2) Domain-specific languages are more precise and expressive and help describe one concrete domain.
+The distinction between GPL and DSL is rather subtle. If one takes UML and applies it to the domain of all software systems it can also be regarded as DSL. Another point arises whether one should use a general-purpose-modeling language or write a custom small DSL for modeling. The benefit of having a custom DSL is reduced to a minimum if it repeats many flavors of GPM languages.</t>
+  </si>
+  <si>
+    <t>"@article{brambilla2017model,
+  title={Model-driven software engineering in practice},
+  author={Brambilla, Marco and Cabot, Jordi and Wimmer, Manuel},
+  journal={Synthesis lectures on software engineering},
+  volume={3},
+  number={1},
+  pages={1--207},
+  year={2017},
+  publisher={Morgan \&amp; Claypool Publishers}
+}"</t>
+  </si>
+  <si>
+    <t>Book about mde with many useful concepts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Systematic Approach to Domain-Specific Language Design Using UML </t>
+  </si>
+  <si>
+    <t>The author argues domain languages significantly foster the software development cycle by focusing first on domain-specific concepts.
+Even though new domain languages are introduced nowadays, they gain little acceptance. The biggest observed issue in the industry is that domain-specific languages do not have adequate tool support required for developing software systems. Comprehensive language would possess a compiler, debugger, and integration for transformation tools. Moreover, domain-specific languages lack support and integration of third-party libraries, unlike general-purpose languages.
+At the same time, using a generalized language imposes some limitations on a programmer to describe a domain. A developer is at least limited to the syntax and metamodel of a language.
+Even though UML allows specifying new language families via profiles, stereotypes, and tagged values, many researchers criticized its initial implementation. This author claims that the newly introduced elements are vague and not flexible enough to provide full expressiveness for a domain.</t>
+  </si>
+  <si>
+    <t>"@inproceedings{selic2007systematic,
+  title={A systematic approach to domain-specific language design using UML},
+  author={Selic, Bran},
+  booktitle={10th IEEE International Symposium on Object and Component-Oriented Real-Time Distributed Computing (ISORC'07)},
+  pages={2--9},
+  year={2007},
+  organization={IEEE}
+}"</t>
   </si>
 </sst>
 </file>
@@ -367,7 +484,48 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="20">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -528,15 +686,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8285077E-5915-4057-BA77-1D27902F310A}" name="Table1" displayName="Table1" ref="A1:F7" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8285077E-5915-4057-BA77-1D27902F310A}" name="Table1" displayName="Table1" ref="A1:F7" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16" totalsRowBorderDxfId="15">
   <autoFilter ref="A1:F7" xr:uid="{BA718EE1-49D7-4650-B037-0771614423BF}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{FF3B8A2A-F932-41FA-95FE-F39F73C1F2C4}" name="Citation" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{9B6745B4-27F0-426A-8DDC-565EB29CD89F}" name="Paper" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{07897410-23B2-4D10-BE84-96D70F98FBC6}" name="Goals" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{A1146B1C-F33C-432E-90B6-E265AC99A77B}" name="Used methods" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{04662BCC-AEE1-4C61-887F-F2AF7BAE3722}" name="Results" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{0DF0A271-EB9F-4F3F-959F-4DECC9AAB759}" name="Why important (one sentence)" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{FF3B8A2A-F932-41FA-95FE-F39F73C1F2C4}" name="Citation" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{9B6745B4-27F0-426A-8DDC-565EB29CD89F}" name="Paper" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{07897410-23B2-4D10-BE84-96D70F98FBC6}" name="Goals" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{A1146B1C-F33C-432E-90B6-E265AC99A77B}" name="Used methods" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{04662BCC-AEE1-4C61-887F-F2AF7BAE3722}" name="Results" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{0DF0A271-EB9F-4F3F-959F-4DECC9AAB759}" name="Why important (one sentence)" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{822ADA59-34C7-4394-AE31-5D8AD6802D70}" name="Table3" displayName="Table3" ref="A1:F6" totalsRowShown="0" headerRowDxfId="7" dataDxfId="0" headerRowBorderDxfId="8">
+  <autoFilter ref="A1:F6" xr:uid="{DBC3082E-8AB2-4060-B752-8823303D327C}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{04A3358C-38AC-41A2-9EF8-F78CF5E86A8B}" name="Citation" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{07437842-31FC-44BC-A480-C79738F8C3E8}" name="Paper" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{C6E7F471-DA9B-4BD0-8B32-356D9F201A60}" name="Goals" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{FBBB0C1C-EB51-4A40-AA30-BEA588E8E954}" name="Used methods" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{B26D925F-D757-43CA-B039-C3186A8D2D00}" name="Results" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{19B8339E-AF8E-4C2D-9935-DF88EDB3038A}" name="Why important (one sentence)" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -807,8 +980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -972,28 +1145,130 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CF1A488-2851-4C66-A331-30E6C95E0D1D}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" customWidth="1"/>
+    <col min="4" max="4" width="15.77734375" customWidth="1"/>
+    <col min="5" max="5" width="67.77734375" customWidth="1"/>
+    <col min="6" max="6" width="27.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="331.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3F4F4E1-D1E9-4F42-9C7C-394B46E3D0E8}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
One more subchapter is ready
</commit_message>
<xml_diff>
--- a/papers/references.xlsx
+++ b/papers/references.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ansk\github\Master-s-thesis\papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA301A94-51CA-4493-8B9D-102B6FBEFE3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85CDE443-7683-4D90-BC2B-DE9251FCBA39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model-driven engineering" sheetId="1" r:id="rId1"/>
     <sheet name="Models and metamodels" sheetId="2" r:id="rId2"/>
+    <sheet name="Multilevel models" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="83">
   <si>
     <t>Citation</t>
   </si>
@@ -335,6 +336,92 @@
   </si>
   <si>
     <t>A metamodel hierarchy is shown in Figure 1. On its top level is a meta-meta model or a graph schema of a language. This level hosts concepts and rules for the level below. The concept that might be difficult to grasp at first glance is that the M3 level is self-descriptive. Many M3 languages can be used to describe themselves on the M2 level. The property of being self-descriptive or lifted as stated here [] is the reason why there is no more level in a classical metamodeling hierarchy. M2 level contains language specifications. For example, UML concepts are defined at this level. Level M1 has software classes or application concepts. The M0 level contains real objects that are instances of the M1 level. Also, there is the M-1 level which is a real-world where software objects have digital twins of real objects. Digital twin takes the state of a real object at runtime.</t>
+  </si>
+  <si>
+    <t>Answer the following questions:</t>
+  </si>
+  <si>
+    <t>1) what is it</t>
+  </si>
+  <si>
+    <t>2) why it is needed</t>
+  </si>
+  <si>
+    <t>3) advantages against traditional modeling</t>
+  </si>
+  <si>
+    <t>4) limitations or disadvantages</t>
+  </si>
+  <si>
+    <t>Modeling Language Extension in the Enterprise Systems Domain</t>
+  </si>
+  <si>
+    <t>The Essence of Multilevel Metamodeling</t>
+  </si>
+  <si>
+    <t>On the Execution of Deep Models</t>
+  </si>
+  <si>
+    <t>Flexible Deep Modeling with Melanee</t>
+  </si>
+  <si>
+    <t>"@inproceedings{atkinson2013modeling,
+  title={Modeling language extension in the enterprise systems domain},
+  author={Atkinson, Colin and Gerbig, Ralph and Fritzsche, Mathias},
+  booktitle={2013 17th IEEE International Enterprise Distributed Object Computing Conference},
+  pages={49--58},
+  year={2013},
+  organization={IEEE}
+}"</t>
+  </si>
+  <si>
+    <t>"@inproceedings{atkinson2001essence,
+  title={The essence of multilevel metamodeling},
+  author={Atkinson, Colin and K{\"u}hne, Thomas},
+  booktitle={International Conference on the Unified Modeling Language},
+  pages={19--33},
+  year={2001},
+  organization={Springer}
+}"</t>
+  </si>
+  <si>
+    <t>"@inproceedings{madoc43510,
+        language = {English},
+       publisher = {RWTH Aachen},
+           title = {On the execution of deep models},
+           pages = {28--33},
+         address = {Aachen, Germany},
+         journal = {CEUR Workshop Proceedings},
+          author = {Colin Atkinson and Ralph Gerbig and Noah Metzger},
+          editor = {Tanja Mayerhofer},
+       booktitle = {EXE 2015 :  Proceedings of the 1st International Workshop on Executable Modeling co-located with ACM/IEEE 18th International Conference on Model Driven Engineering Languages and Systems (MODELS 2015) Ottawa, Canada, September 27, 2015},
+          volume = {1560},
+            year = {2015},
+             url = {https://madoc.bib.uni-mannheim.de/43510/}
+}"</t>
+  </si>
+  <si>
+    <t>"@article{atkinson2016flexible,
+  title={Flexible deep modeling with melanee},
+  author={Atkinson, Colin and Gerbig, Ralph},
+  journal={Modellierung 2016-Workshopband},
+  year={2016},
+  publisher={Gesellschaft f{\"u}r Informatik eV}
+}"</t>
+  </si>
+  <si>
+    <t>Analyse current approaches for language extension and propose the own one</t>
+  </si>
+  <si>
+    <t>The demand to enhance tools in the presence of changing requirements is rising. However, the obstacles are the metamodels to define such languages because they do not support extension with their current architecture. Some workarounds are a common practice to avoid such limitations that increase the complexity of architecture and prevent the following of enterprise principles.
+As summarized here, three techniques to overcome the problems of tool's co-evolutions as well as their advantages and disadvantages are present below:
+	1) Direct metamodel enhancement. Problems: many frameworks do not allow changing a metamodel at runtime, and many tools that use the metamodel for defining concepts do not update dynamically without redeployment.
+	2) M2 level extension of a language when instead of enriching the metamodel, embedded mechanisms are provided for users to expand a framework. Problems with process compatibility. If two frameworks define two equal concepts on the M2 level then those concepts cannot be wired interchangeably without being introduced on the M3 level.
+	3) Model annotation approach. It enables the separation of an extended language from a language used for model enrichment. The newly introduced models are then linked to a target model without its direct modifications. However, first of all, it requires the support and maintenance of two different models. Moreover, some model elements must be duplicated which makes it cumbersome to keep two models synchronized.</t>
+  </si>
+  <si>
+    <t>Another problem of traditional metamodel hierarchy is its inability to naturally model a domain that cannot be expressed within only two levels provided by modern modeling frameworks. Moreover, modifications and dynamically adding new features to a system without redeploying it are impossible.
+The limitations mentioned above can be eliminated with the use of deep models. This concept is based on the Orthogonal Classification Architecture (OCA). This architecture defines two orthogonal dimensions with two different views on a model. Thus, the language dimension views a model as a part of a classical metamodel hierarchy. In its turn, the ontological dimension contains the classification of a domain. An example is illustrated in the picture below. Then you should define language levels. To highlight the idea that elements of an ontological model hierarchy have both class and instance features, the term clabject is introduced. Moreover, the term "potency" is defined that shows over how many levels of a certain element can be instantiated.</t>
   </si>
 </sst>
 </file>
@@ -510,7 +597,157 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="31">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -712,30 +949,45 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8285077E-5915-4057-BA77-1D27902F310A}" name="Table1" displayName="Table1" ref="A1:F7" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16" totalsRowBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8285077E-5915-4057-BA77-1D27902F310A}" name="Table1" displayName="Table1" ref="A1:F7" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <autoFilter ref="A1:F7" xr:uid="{BA718EE1-49D7-4650-B037-0771614423BF}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{FF3B8A2A-F932-41FA-95FE-F39F73C1F2C4}" name="Citation" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{9B6745B4-27F0-426A-8DDC-565EB29CD89F}" name="Paper" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{07897410-23B2-4D10-BE84-96D70F98FBC6}" name="Goals" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{A1146B1C-F33C-432E-90B6-E265AC99A77B}" name="Used methods" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{04662BCC-AEE1-4C61-887F-F2AF7BAE3722}" name="Results" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{0DF0A271-EB9F-4F3F-959F-4DECC9AAB759}" name="Why important (one sentence)" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{FF3B8A2A-F932-41FA-95FE-F39F73C1F2C4}" name="Citation" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{9B6745B4-27F0-426A-8DDC-565EB29CD89F}" name="Paper" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{07897410-23B2-4D10-BE84-96D70F98FBC6}" name="Goals" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{A1146B1C-F33C-432E-90B6-E265AC99A77B}" name="Used methods" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{04662BCC-AEE1-4C61-887F-F2AF7BAE3722}" name="Results" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{0DF0A271-EB9F-4F3F-959F-4DECC9AAB759}" name="Why important (one sentence)" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{822ADA59-34C7-4394-AE31-5D8AD6802D70}" name="Table3" displayName="Table3" ref="A1:F7" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{822ADA59-34C7-4394-AE31-5D8AD6802D70}" name="Table3" displayName="Table3" ref="A1:F7" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18">
   <autoFilter ref="A1:F7" xr:uid="{DBC3082E-8AB2-4060-B752-8823303D327C}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{04A3358C-38AC-41A2-9EF8-F78CF5E86A8B}" name="Citation" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{07437842-31FC-44BC-A480-C79738F8C3E8}" name="Paper" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{C6E7F471-DA9B-4BD0-8B32-356D9F201A60}" name="Goals" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{FBBB0C1C-EB51-4A40-AA30-BEA588E8E954}" name="Used methods" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{B26D925F-D757-43CA-B039-C3186A8D2D00}" name="Results" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{19B8339E-AF8E-4C2D-9935-DF88EDB3038A}" name="Why important (one sentence)" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{04A3358C-38AC-41A2-9EF8-F78CF5E86A8B}" name="Citation" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{07437842-31FC-44BC-A480-C79738F8C3E8}" name="Paper" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{C6E7F471-DA9B-4BD0-8B32-356D9F201A60}" name="Goals" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{FBBB0C1C-EB51-4A40-AA30-BEA588E8E954}" name="Used methods" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{B26D925F-D757-43CA-B039-C3186A8D2D00}" name="Results" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{19B8339E-AF8E-4C2D-9935-DF88EDB3038A}" name="Why important (one sentence)" dataDxfId="11"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DFDAF967-C688-4C03-A27F-5FD297F6AB37}" name="Table4" displayName="Table4" ref="A7:F11" totalsRowShown="0" headerRowDxfId="7" dataDxfId="0" headerRowBorderDxfId="9" tableBorderDxfId="10" totalsRowBorderDxfId="8">
+  <autoFilter ref="A7:F11" xr:uid="{5E47718A-97F9-432C-B83E-51A5A64721F9}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{42E1F1A7-0EDD-487C-B287-C83C32773D6F}" name="Citation" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{85E079A5-BC8D-4735-863E-AE69887C7784}" name="Paper" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{1998B378-71BB-42A6-BD3B-B6DB7CF49B9F}" name="Goals" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{E40C5699-D930-4E6B-80D1-80A1E126EA5E}" name="Used methods" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{E32B528D-F116-49F3-9313-33D9BB463AAC}" name="Results" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{7AA69EB9-56A4-470C-B997-C9AF00351BC6}" name="Why important (one sentence)" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1173,8 +1425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CF1A488-2851-4C66-A331-30E6C95E0D1D}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1322,4 +1574,129 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{171206E4-2EA6-4B1F-83FB-DEC77FFB9355}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.5546875" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" customWidth="1"/>
+    <col min="5" max="5" width="66.6640625" customWidth="1"/>
+    <col min="6" max="6" width="32" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="1:6" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="1:6" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" spans="1:6" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Must still process all the info about models at runtime
</commit_message>
<xml_diff>
--- a/papers/references.xlsx
+++ b/papers/references.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ansk\github\Master-s-thesis\papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85CDE443-7683-4D90-BC2B-DE9251FCBA39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{432AB639-5629-4368-8314-0C94AC562B9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model-driven engineering" sheetId="1" r:id="rId1"/>
     <sheet name="Models and metamodels" sheetId="2" r:id="rId2"/>
     <sheet name="Multilevel models" sheetId="3" r:id="rId3"/>
+    <sheet name="Models@runtime" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="98">
   <si>
     <t>Citation</t>
   </si>
@@ -422,6 +423,118 @@
   <si>
     <t>Another problem of traditional metamodel hierarchy is its inability to naturally model a domain that cannot be expressed within only two levels provided by modern modeling frameworks. Moreover, modifications and dynamically adding new features to a system without redeploying it are impossible.
 The limitations mentioned above can be eliminated with the use of deep models. This concept is based on the Orthogonal Classification Architecture (OCA). This architecture defines two orthogonal dimensions with two different views on a model. Thus, the language dimension views a model as a part of a classical metamodel hierarchy. In its turn, the ontological dimension contains the classification of a domain. An example is illustrated in the picture below. Then you should define language levels. To highlight the idea that elements of an ontological model hierarchy have both class and instance features, the term clabject is introduced. Moreover, the term "potency" is defined that shows over how many levels of a certain element can be instantiated.</t>
+  </si>
+  <si>
+    <t>Systematic literature review of the objectives, techniques, kinds,
+and architectures of models at runtime</t>
+  </si>
+  <si>
+    <t>"@article{szvetits2016systematic,
+  title={Systematic literature review of the objectives, techniques, kinds, and architectures of models at runtime},
+  author={Szvetits, Michael and Zdun, Uwe},
+  journal={Software \&amp; Systems Modeling},
+  volume={15},
+  number={1},
+  pages={31--69},
+  year={2016},
+  publisher={Springer}
+}"</t>
+  </si>
+  <si>
+    <t>Page 9 has a nice table with application of models at runtime. It might be useful to refer to it later on;</t>
+  </si>
+  <si>
+    <t>An Eclipse Modelling Framework Alternativeto Meet the Models@Runtime Requirements</t>
+  </si>
+  <si>
+    <t>"@inproceedings{fouquet2012eclipse,
+  title={An eclipse modelling framework alternative to meet the models@ runtime requirements},
+  author={Fouquet, Fran{\c{c}}ois and Nain, Gr{\'e}gory and Morin, Brice and Daubert, Erwan and Barais, Olivier and Plouzeau, No{\"e}l and J{\'e}z{\'e}quel, Jean-Marc},
+  booktitle={International conference on model driven engineering languages and systems},
+  pages={87--101},
+  year={2012},
+  organization={Springer}
+}"</t>
+  </si>
+  <si>
+    <t>Models@Runtime aims at taming the complexity of softwaredynamic adaptation by pushing further the idea of reflection and con-sidering the reflection layer as a first-class modeling space. A naturalapproach to Models@Runtime is to use MDE techniques, in particularthose based on the Eclipse Modeling Framework;
+A natural approach to Models@Runtime is to use MDE techniques, in par-ticular those based on the Eclipse Modeling Framework (EMF); More precisely, the goal of Models@Runtime is to enable the con-tinuous design, evolution, verification of eternal running software systems</t>
+  </si>
+  <si>
+    <t>Models@Runtime: The Development and Re-Configuration Management of Python Applications Using Formal Methods</t>
+  </si>
+  <si>
+    <t>Runtime models can be regarded as a reflexive layer causally connected with the underlying system. Hence, every change in the runtime model involves a change in the reflected system, and vice versa;         
+ the main advantage of models@runtime is the use of an abstraction of the running software in the form of a model to enable its reconfiguration by changing its behavior while the software is still running; 
+The system and its corresponding model are causally connected, so the model is updated according to the current state of the system, and vice versa;
+The models@runtime offers new techniques to deal with the dynamic adaptation of systems and satisfy the increasing complexity of user
+requirements. Therefore, in our work, it enables the dynamic reconfiguration management of Python applications.
+The models@runtime vision consists in the use of models not only at the design time but also during runtime. The underlying systems and their corresponding models evolve together and affect each other during the execution of these systems. The models@runtime paradigm enables the running systems to cope with the dynamic change of environments
+and satisfy the complex requirements of users;
+Model-Driven Engineering (MDE) increases the importance of the notion of models because they are considered central artifacts in the development process. One of the challenges of the MDE community is to use models, as central artifacts, at runtime, to cope with dynamic aspects of ever-changing software and its environment [4], which inspired the notion of models@runtime;
+For instance, regarding the grading example, the method to determine successful students may unexpectedly change. For instance, many universities have changed their assessment methods during the SARS-CoV-2 pandemic (COVID-19). In Algeria, for example,
+a compensation system is used considering the average of both semesters. Thus, a pass is awarded to students with a total average for both semesters of 50 or above. Developers need to adapt the program to this new requirement. In an ordinary software development process, developers have to stop the execution, change the model, generate the code, and re-start the execution. However, using the models@runtime technique, developers could perform this change without stopping the execution. That is, they would be able to execute models using an execution engine where an engine reflecting the software
+execution enables the developer to monitor the execution. If the execution engine is able to automatically perform the change in the running instance, developers can monitor the change itself. In addition, a better connection between the design model and the execution can provide certain advantages, such as being able to see the execution state in order to inspect the value of variables before and after the change. Another benefit can be achieved by the adoption of a loosely coupled solution between the model and the execution, which can improve the system flexibility and allow for its deployment in distributed systems;</t>
+  </si>
+  <si>
+    <t>"@article{bouhamed2021models,
+  title={Models@ Runtime: The Development and Re-Configuration Management of Python Applications Using Formal Methods},
+  author={Bouhamed, Mohammed Mounir and D{\'\i}az, Gregorio and Chaoui, Allaoua and Kamel, Oussama and Nouara, Radouane},
+  journal={Applied Sciences},
+  volume={11},
+  number={20},
+  pages={9743},
+  year={2021},
+  publisher={MDPI}
+}"</t>
+  </si>
+  <si>
+    <t>A Reference Architecture and Roadmap for Models@run.time Systems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There is, however, a growing need for more flexible adaptive systems, able to cope with unanticipated situations, still without jeopardizing safety properties. This is typically the case of Cyber-Physical Systems (CPS) as described in Section 6. Hence, new approaches are needed to enable unanticipated adaptations while ensuring guarantees. This is, in our
+opinion, the ultimate purpose of models@run.time.
+models@run.time systems provide and use manageable reflection, which is characterized to be tractable and predictable and by this overcomes the limitation of classic reflection on code, which faces the problem of undecidability.
+Systems, according to the models@run.time paradigm, are based on the reflection principles.In practice however, reflection is a powerful yet hazardous process (see for example the drawbacks of the Java reflection API, clearly reported by Oracle3), since it provides no support to “preview” what will be the result of an adaptation. Basically, erroneous adaptation based on reflection can only be detected a posteriori, or even post mortem if the rollback mechanisms were not able to put the system back to a safe state.
+We perceive reflection, modeling and separation of concerns as the three main pillars to achieve models@run.time and make future software systems able of intelligent thinking, i.e., abstract, predictive reflection
+Each models@run.time system comprises three layers, comparable to the layers of Kramer and Magee [KM09]. From bottom to top these are: – a base layer comprising models of the managed system, – a configuration management layer comprising active components of the system realizing the feedback loop on the managed system and – a goal management layer comprising models of the system’s goals, realizing an internal feedback loop between the goal management layer as managing element and the configuration management layer as managed element.
+The base layer comprises four types of models, which are abstractions of specific aspects of the system for a given purpose: Context Models contain relevant information about the current state of the managed system’s environment, e.g., the current temperature, or higher level context information such as an alert information derived by aggregating or interpreting the information of different sensors.
+Configuration Models express the current configuration of the managed system, i.e., its current state. Current models@run.time approaches usually provide an architectural view on the managed system (i.e., which services are currently deployed and running on which resources). Both, configuration and context models, cover the abstracted runtime state subject to tractable, predictive reflection.
+Capability Models describe the features available to influence the managed system (e.g., whether software components can be added/removed and rebound, whether parameters of system components can be adjusted), which actuators are available and how they can affect the environment. Typically this model is rather static and depends on the underlying infrastructure. However, this model can be updated, e.g., after a new actuator has been added in the system
+Plan Models describe a set of actions (according to the capability models) to be performed by the system to realize an adaptation. They represent reconfiguration or action scripts, which describe how the managed system shall be reconfigured and how the actuators of the managed systems shall be used to effect the environment.
+The configuration management layer contains the active entities of a models@run.time system, which make use of the models of the base layer. This layer typically comprises a reasoner, an analyzer and optionally a learner.
+The reasoner’s evaluates alternative future configurations of the system. This includes (1) to realize the predictive reflection, (2) to identify the best configuration w.r.t. the goals specified on the top layer, and (3) to derive reconfiguration or action plans to establish the envisioned system configuration.
+The analyzer has two tasks. First, the analyzer has to detect whether the whole system (i.e., managed and managing system) should be re-evaluated. To do so, the current system state has to be evaluated against the system’s goals. If the current system state deviates from the goals, the analyzer will trigger the reasoner, to compute a reconfiguration plan. Second, the analyzer further abstracts the information contained in the models of the base layer. This raises the level of abstraction of the models and, in turn, to lower the complexity of predictive reflection.
+The learner has two tasks, too. On the one side, the learner is responsible to keep the models of the base layer synchronized with the system. Thus, the learner utilizes the managed systems sensors to capture the environment’s state and continuously observes the managed system itself to update the context and configuration model on the base layer. On the other side, the learner can observe the reasoner to detect, whether the decisions of the reasoner are beneficial on the long run or not. </t>
+  </si>
+  <si>
+    <t>"@incollection{assmann2014reference,
+  title={A reference architecture and roadmap for models@ run. time systems},
+  author={A{\ss}mann, Uwe and G{\"o}tz, Sebastian and J{\'e}z{\'e}quel, Jean-Marc and Morin, Brice and Trapp, Mario},
+  booktitle={Models@ run. time},
+  pages={1--18},
+  year={2014},
+  publisher={Springer}
+}"</t>
+  </si>
+  <si>
+    <t>The kind of models used at runtime can be classified by (1) their purpose—predictive, prescriptive, constructive, or descriptive; (2) their underlying modeling languages—for example, the 14 UML 2.2 structural and behavioral diagrams, State-charts, Petri Nets, and logic based models (e.g., Temporal Logics); and (3) the aspects they describe—data structure, task or process state, I/O behavior, or interaction pattern.
+One of the main principles of using M@RT for assurance is to exploit the causal connection [Mae87] between the model and the system under development at runtime.
+We argue that M@RT provide abstractions that are essential to support the feedback loops that control the three levels of dynamics identified in SASs. From this perspective, M@RT (cf. Figure 1) could be developed specifically for each level of dynamics to support the control objectives manager, adaptation controller, and the monitoring system. The figure also shows the interactions between these models and the respective subsystems in an SAS.
+At the Control Objectives level, M@RT represent requirements specifications subject to assurance in the form of functional and non-functional requirements. – At the Adaptation level, M@RT represent states of the managed system, adaptation plans and their relationships with the assurance specifications. – At the Monitoring level, M@RT represent context entities, monitoring requirements, as well as monitoring strategies and their relationships with assurance criteria and adaptation models. Most importantly, M@RT at these levels must have efficient and effective methods of inter-level interaction since changes in requirement specifications may trigger changes at both the adaptation and the monitoring levels, as well as in the associated runtime models. Similarly, changes in adaptation models may imply changes in monitoring strategies or context entity models. In any case, M@RT at the adaptation and monitoring levels must maintain an explicit mapping to the models defined at the control objectives level that specify the requirements.</t>
+  </si>
+  <si>
+    <t>Using Models at Runtime to Address Assurance for Self-Adaptive Systems</t>
+  </si>
+  <si>
+    <t>"@incollection{cheng2014using,
+  title={Using models at runtime to address assurance for self-adaptive systems},
+  author={Cheng, Betty HC and Eder, Kerstin I and Gogolla, Martin and Grunske, Lars and Litoiu, Marin and M{\"u}ller, Hausi A and Pelliccione, Patrizio and Perini, Anna and Qureshi, Nauman A and Rumpe, Bernhard and others},
+  booktitle={Models@ run. time},
+  pages={101--136},
+  year={2014},
+  publisher={Springer}
+}"</t>
   </si>
 </sst>
 </file>
@@ -552,7 +665,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -593,13 +706,138 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="31">
+  <dxfs count="40">
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -700,6 +938,39 @@
       </border>
     </dxf>
     <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -716,36 +987,6 @@
         <horizontal style="thin">
           <color indexed="64"/>
         </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -949,45 +1190,60 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8285077E-5915-4057-BA77-1D27902F310A}" name="Table1" displayName="Table1" ref="A1:F7" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8285077E-5915-4057-BA77-1D27902F310A}" name="Table1" displayName="Table1" ref="A1:F7" totalsRowShown="0" headerRowDxfId="39" dataDxfId="37" headerRowBorderDxfId="38" tableBorderDxfId="36" totalsRowBorderDxfId="35">
   <autoFilter ref="A1:F7" xr:uid="{BA718EE1-49D7-4650-B037-0771614423BF}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{FF3B8A2A-F932-41FA-95FE-F39F73C1F2C4}" name="Citation" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{9B6745B4-27F0-426A-8DDC-565EB29CD89F}" name="Paper" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{07897410-23B2-4D10-BE84-96D70F98FBC6}" name="Goals" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{A1146B1C-F33C-432E-90B6-E265AC99A77B}" name="Used methods" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{04662BCC-AEE1-4C61-887F-F2AF7BAE3722}" name="Results" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{0DF0A271-EB9F-4F3F-959F-4DECC9AAB759}" name="Why important (one sentence)" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{FF3B8A2A-F932-41FA-95FE-F39F73C1F2C4}" name="Citation" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{9B6745B4-27F0-426A-8DDC-565EB29CD89F}" name="Paper" dataDxfId="33"/>
+    <tableColumn id="5" xr3:uid="{07897410-23B2-4D10-BE84-96D70F98FBC6}" name="Goals" dataDxfId="32"/>
+    <tableColumn id="6" xr3:uid="{A1146B1C-F33C-432E-90B6-E265AC99A77B}" name="Used methods" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{04662BCC-AEE1-4C61-887F-F2AF7BAE3722}" name="Results" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{0DF0A271-EB9F-4F3F-959F-4DECC9AAB759}" name="Why important (one sentence)" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{822ADA59-34C7-4394-AE31-5D8AD6802D70}" name="Table3" displayName="Table3" ref="A1:F7" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{822ADA59-34C7-4394-AE31-5D8AD6802D70}" name="Table3" displayName="Table3" ref="A1:F7" totalsRowShown="0" headerRowDxfId="28" dataDxfId="26" headerRowBorderDxfId="27">
   <autoFilter ref="A1:F7" xr:uid="{DBC3082E-8AB2-4060-B752-8823303D327C}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{04A3358C-38AC-41A2-9EF8-F78CF5E86A8B}" name="Citation" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{07437842-31FC-44BC-A480-C79738F8C3E8}" name="Paper" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{C6E7F471-DA9B-4BD0-8B32-356D9F201A60}" name="Goals" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{FBBB0C1C-EB51-4A40-AA30-BEA588E8E954}" name="Used methods" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{B26D925F-D757-43CA-B039-C3186A8D2D00}" name="Results" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{19B8339E-AF8E-4C2D-9935-DF88EDB3038A}" name="Why important (one sentence)" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{04A3358C-38AC-41A2-9EF8-F78CF5E86A8B}" name="Citation" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{07437842-31FC-44BC-A480-C79738F8C3E8}" name="Paper" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{C6E7F471-DA9B-4BD0-8B32-356D9F201A60}" name="Goals" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{FBBB0C1C-EB51-4A40-AA30-BEA588E8E954}" name="Used methods" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{B26D925F-D757-43CA-B039-C3186A8D2D00}" name="Results" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{19B8339E-AF8E-4C2D-9935-DF88EDB3038A}" name="Why important (one sentence)" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DFDAF967-C688-4C03-A27F-5FD297F6AB37}" name="Table4" displayName="Table4" ref="A7:F11" totalsRowShown="0" headerRowDxfId="7" dataDxfId="0" headerRowBorderDxfId="9" tableBorderDxfId="10" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DFDAF967-C688-4C03-A27F-5FD297F6AB37}" name="Table4" displayName="Table4" ref="A7:F11" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16" totalsRowBorderDxfId="15">
   <autoFilter ref="A7:F11" xr:uid="{5E47718A-97F9-432C-B83E-51A5A64721F9}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{42E1F1A7-0EDD-487C-B287-C83C32773D6F}" name="Citation" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{85E079A5-BC8D-4735-863E-AE69887C7784}" name="Paper" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{1998B378-71BB-42A6-BD3B-B6DB7CF49B9F}" name="Goals" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{E40C5699-D930-4E6B-80D1-80A1E126EA5E}" name="Used methods" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{E32B528D-F116-49F3-9313-33D9BB463AAC}" name="Results" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{7AA69EB9-56A4-470C-B997-C9AF00351BC6}" name="Why important (one sentence)" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{42E1F1A7-0EDD-487C-B287-C83C32773D6F}" name="Citation" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{85E079A5-BC8D-4735-863E-AE69887C7784}" name="Paper" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{1998B378-71BB-42A6-BD3B-B6DB7CF49B9F}" name="Goals" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{E40C5699-D930-4E6B-80D1-80A1E126EA5E}" name="Used methods" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{E32B528D-F116-49F3-9313-33D9BB463AAC}" name="Results" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{7AA69EB9-56A4-470C-B997-C9AF00351BC6}" name="Why important (one sentence)" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4BC5F24D-CAB9-4CFF-9A90-81F0A97CC23D}" name="Table2" displayName="Table2" ref="A1:F9" totalsRowShown="0" headerRowDxfId="7" dataDxfId="0" headerRowBorderDxfId="8">
+  <autoFilter ref="A1:F9" xr:uid="{B5EB7290-80D5-4166-A1AF-2F3EC711E8C0}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{C38A4344-5940-4D1A-954B-B327F67FC51B}" name="Citation" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{21871081-5263-4105-824F-702819BE3257}" name="Paper" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{5EC33F8F-E087-4F09-9973-DCEF253DE1F2}" name="Goals" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{8D925C0B-F22B-4B4B-9CB8-82AF34581EB3}" name="Used methods" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{149BEA12-A580-4BC7-8E8D-1A653C01B43F}" name="Results" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{B4C351CA-7B7B-4C23-A447-B3E32BD05355}" name="Why important (one sentence)" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1258,7 +1514,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -1425,7 +1681,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CF1A488-2851-4C66-A331-30E6C95E0D1D}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="F1" sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
@@ -1580,8 +1836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{171206E4-2EA6-4B1F-83FB-DEC77FFB9355}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1699,4 +1955,144 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C75DB7F1-B501-46CE-AB52-85AC9D327FEE}">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.5546875" customWidth="1"/>
+    <col min="2" max="2" width="18.77734375" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="15.21875" customWidth="1"/>
+    <col min="5" max="5" width="71.88671875" customWidth="1"/>
+    <col min="6" max="6" width="36.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:6" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:6" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Models@run.time subchapter is ready
</commit_message>
<xml_diff>
--- a/papers/references.xlsx
+++ b/papers/references.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ansk\github\Master-s-thesis\papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{432AB639-5629-4368-8314-0C94AC562B9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A3F371-FF88-42E1-AED7-516250735053}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="98">
   <si>
     <t>Citation</t>
   </si>
@@ -457,24 +457,7 @@
 }"</t>
   </si>
   <si>
-    <t>Models@Runtime aims at taming the complexity of softwaredynamic adaptation by pushing further the idea of reflection and con-sidering the reflection layer as a first-class modeling space. A naturalapproach to Models@Runtime is to use MDE techniques, in particularthose based on the Eclipse Modeling Framework;
-A natural approach to Models@Runtime is to use MDE techniques, in par-ticular those based on the Eclipse Modeling Framework (EMF); More precisely, the goal of Models@Runtime is to enable the con-tinuous design, evolution, verification of eternal running software systems</t>
-  </si>
-  <si>
     <t>Models@Runtime: The Development and Re-Configuration Management of Python Applications Using Formal Methods</t>
-  </si>
-  <si>
-    <t>Runtime models can be regarded as a reflexive layer causally connected with the underlying system. Hence, every change in the runtime model involves a change in the reflected system, and vice versa;         
- the main advantage of models@runtime is the use of an abstraction of the running software in the form of a model to enable its reconfiguration by changing its behavior while the software is still running; 
-The system and its corresponding model are causally connected, so the model is updated according to the current state of the system, and vice versa;
-The models@runtime offers new techniques to deal with the dynamic adaptation of systems and satisfy the increasing complexity of user
-requirements. Therefore, in our work, it enables the dynamic reconfiguration management of Python applications.
-The models@runtime vision consists in the use of models not only at the design time but also during runtime. The underlying systems and their corresponding models evolve together and affect each other during the execution of these systems. The models@runtime paradigm enables the running systems to cope with the dynamic change of environments
-and satisfy the complex requirements of users;
-Model-Driven Engineering (MDE) increases the importance of the notion of models because they are considered central artifacts in the development process. One of the challenges of the MDE community is to use models, as central artifacts, at runtime, to cope with dynamic aspects of ever-changing software and its environment [4], which inspired the notion of models@runtime;
-For instance, regarding the grading example, the method to determine successful students may unexpectedly change. For instance, many universities have changed their assessment methods during the SARS-CoV-2 pandemic (COVID-19). In Algeria, for example,
-a compensation system is used considering the average of both semesters. Thus, a pass is awarded to students with a total average for both semesters of 50 or above. Developers need to adapt the program to this new requirement. In an ordinary software development process, developers have to stop the execution, change the model, generate the code, and re-start the execution. However, using the models@runtime technique, developers could perform this change without stopping the execution. That is, they would be able to execute models using an execution engine where an engine reflecting the software
-execution enables the developer to monitor the execution. If the execution engine is able to automatically perform the change in the running instance, developers can monitor the change itself. In addition, a better connection between the design model and the execution can provide certain advantages, such as being able to see the execution state in order to inspect the value of variables before and after the change. Another benefit can be achieved by the adoption of a loosely coupled solution between the model and the execution, which can improve the system flexibility and allow for its deployment in distributed systems;</t>
   </si>
   <si>
     <t>"@article{bouhamed2021models,
@@ -492,22 +475,6 @@
     <t>A Reference Architecture and Roadmap for Models@run.time Systems</t>
   </si>
   <si>
-    <t xml:space="preserve">There is, however, a growing need for more flexible adaptive systems, able to cope with unanticipated situations, still without jeopardizing safety properties. This is typically the case of Cyber-Physical Systems (CPS) as described in Section 6. Hence, new approaches are needed to enable unanticipated adaptations while ensuring guarantees. This is, in our
-opinion, the ultimate purpose of models@run.time.
-models@run.time systems provide and use manageable reflection, which is characterized to be tractable and predictable and by this overcomes the limitation of classic reflection on code, which faces the problem of undecidability.
-Systems, according to the models@run.time paradigm, are based on the reflection principles.In practice however, reflection is a powerful yet hazardous process (see for example the drawbacks of the Java reflection API, clearly reported by Oracle3), since it provides no support to “preview” what will be the result of an adaptation. Basically, erroneous adaptation based on reflection can only be detected a posteriori, or even post mortem if the rollback mechanisms were not able to put the system back to a safe state.
-We perceive reflection, modeling and separation of concerns as the three main pillars to achieve models@run.time and make future software systems able of intelligent thinking, i.e., abstract, predictive reflection
-Each models@run.time system comprises three layers, comparable to the layers of Kramer and Magee [KM09]. From bottom to top these are: – a base layer comprising models of the managed system, – a configuration management layer comprising active components of the system realizing the feedback loop on the managed system and – a goal management layer comprising models of the system’s goals, realizing an internal feedback loop between the goal management layer as managing element and the configuration management layer as managed element.
-The base layer comprises four types of models, which are abstractions of specific aspects of the system for a given purpose: Context Models contain relevant information about the current state of the managed system’s environment, e.g., the current temperature, or higher level context information such as an alert information derived by aggregating or interpreting the information of different sensors.
-Configuration Models express the current configuration of the managed system, i.e., its current state. Current models@run.time approaches usually provide an architectural view on the managed system (i.e., which services are currently deployed and running on which resources). Both, configuration and context models, cover the abstracted runtime state subject to tractable, predictive reflection.
-Capability Models describe the features available to influence the managed system (e.g., whether software components can be added/removed and rebound, whether parameters of system components can be adjusted), which actuators are available and how they can affect the environment. Typically this model is rather static and depends on the underlying infrastructure. However, this model can be updated, e.g., after a new actuator has been added in the system
-Plan Models describe a set of actions (according to the capability models) to be performed by the system to realize an adaptation. They represent reconfiguration or action scripts, which describe how the managed system shall be reconfigured and how the actuators of the managed systems shall be used to effect the environment.
-The configuration management layer contains the active entities of a models@run.time system, which make use of the models of the base layer. This layer typically comprises a reasoner, an analyzer and optionally a learner.
-The reasoner’s evaluates alternative future configurations of the system. This includes (1) to realize the predictive reflection, (2) to identify the best configuration w.r.t. the goals specified on the top layer, and (3) to derive reconfiguration or action plans to establish the envisioned system configuration.
-The analyzer has two tasks. First, the analyzer has to detect whether the whole system (i.e., managed and managing system) should be re-evaluated. To do so, the current system state has to be evaluated against the system’s goals. If the current system state deviates from the goals, the analyzer will trigger the reasoner, to compute a reconfiguration plan. Second, the analyzer further abstracts the information contained in the models of the base layer. This raises the level of abstraction of the models and, in turn, to lower the complexity of predictive reflection.
-The learner has two tasks, too. On the one side, the learner is responsible to keep the models of the base layer synchronized with the system. Thus, the learner utilizes the managed systems sensors to capture the environment’s state and continuously observes the managed system itself to update the context and configuration model on the base layer. On the other side, the learner can observe the reasoner to detect, whether the decisions of the reasoner are beneficial on the long run or not. </t>
-  </si>
-  <si>
     <t>"@incollection{assmann2014reference,
   title={A reference architecture and roadmap for models@ run. time systems},
   author={A{\ss}mann, Uwe and G{\"o}tz, Sebastian and J{\'e}z{\'e}quel, Jean-Marc and Morin, Brice and Trapp, Mario},
@@ -518,12 +485,6 @@
 }"</t>
   </si>
   <si>
-    <t>The kind of models used at runtime can be classified by (1) their purpose—predictive, prescriptive, constructive, or descriptive; (2) their underlying modeling languages—for example, the 14 UML 2.2 structural and behavioral diagrams, State-charts, Petri Nets, and logic based models (e.g., Temporal Logics); and (3) the aspects they describe—data structure, task or process state, I/O behavior, or interaction pattern.
-One of the main principles of using M@RT for assurance is to exploit the causal connection [Mae87] between the model and the system under development at runtime.
-We argue that M@RT provide abstractions that are essential to support the feedback loops that control the three levels of dynamics identified in SASs. From this perspective, M@RT (cf. Figure 1) could be developed specifically for each level of dynamics to support the control objectives manager, adaptation controller, and the monitoring system. The figure also shows the interactions between these models and the respective subsystems in an SAS.
-At the Control Objectives level, M@RT represent requirements specifications subject to assurance in the form of functional and non-functional requirements. – At the Adaptation level, M@RT represent states of the managed system, adaptation plans and their relationships with the assurance specifications. – At the Monitoring level, M@RT represent context entities, monitoring requirements, as well as monitoring strategies and their relationships with assurance criteria and adaptation models. Most importantly, M@RT at these levels must have efficient and effective methods of inter-level interaction since changes in requirement specifications may trigger changes at both the adaptation and the monitoring levels, as well as in the associated runtime models. Similarly, changes in adaptation models may imply changes in monitoring strategies or context entity models. In any case, M@RT at the adaptation and monitoring levels must maintain an explicit mapping to the models defined at the control objectives level that specify the requirements.</t>
-  </si>
-  <si>
     <t>Using Models at Runtime to Address Assurance for Self-Adaptive Systems</t>
   </si>
   <si>
@@ -535,6 +496,25 @@
   year={2014},
   publisher={Springer}
 }"</t>
+  </si>
+  <si>
+    <t>Models at runtime aim to facilitate the process of dynamically adding new requirements to software by adding an extra reflection level that maps a model to the underlying software. As the author states, models at runtime make use of MDE principles.
+Models at runtime aim to blur the distinction between software design, its evolution, and execution.</t>
+  </si>
+  <si>
+    <t>Runtime modeling connects software with its abstraction to bidirectionally synchronize an artifact with its reflection. Consequently, it lets to reduce the scheduled downtime of a system since semantic changes and behavior modification happen at runtime. 
+Continuing the main idea of MDE to view models as the most important artifacts during development, models@runtime encourages the use of models not only to design software but also during its execution. Therefore, the running system and its model evolve concurrently. 
+An example that showcases one of the advantages is described below. Consider a system the domain diagram of which is present below. It is not uncommon that after some time, a new requirement is added. In a classical scenario, a development team would have to stop the software, adapt the domain model, regenerate code if needed and deploy the system again. All those cumbersome stages can be avoided by using models at runtime to adapt the domain model on-the-fly. In can be achieved by running models using an execution engine that reflects the current state of a system.</t>
+  </si>
+  <si>
+    <t>There is an increasing demand for self-adaptive systems that can deal with unexpected software changes. As stated here, the three main pillars of models at runtime are modeling, separation of concerns, and reflection.
+The architecture of a model at runtime system is depicted in figure 1. According to the source, it consists of three interrelated parts.
+The first level entitles the models of a target system. It has four model subtypes that abstract the target system. Context models contain the current state of the system environment. Configuration models depict the architectural outlook on the running system. Capability models contain attributes to manage the target system. Even though this model is mostly static and depends on the running infrastructure, it still can be updated after a new component enters a system. The last type of model is a planning model that contains instructions on embedding new components into a target system.
+The next level serves configurational purposes and includes system components that enable feedback interconnection between this management level and the level below. It has active entities such as a reasoner and analyzer to manipulate the models defined on a base level. The reasoner reasons about the configuration state of the system in the future. The analyzer checks whether the target system state corresponds to the goals of the system. If it is not the case, then the analyzer fires a reasoner to reevaluate the configuration. Optionally, a learner can be defined on this level to maintain the synchronization between the models of the base level with the target system and check the usefulness of the reasoner's statements.
+The top level comprises goal-related models of a system and enables connection with the configuration management layer. Those types of models are fed by the reasoner to check if the goals can be fulfilled. It is worth mentioning, that such models tend to evolve over time in the presence of new requirements and goals.</t>
+  </si>
+  <si>
+    <t>The classification of used models at runtime contains three categories. Namely, models can be categorized by the purpose of their use, the language by which they are constructed, and, finally, by the area they represent.</t>
   </si>
 </sst>
 </file>
@@ -703,11 +683,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -716,6 +696,20 @@
   <dxfs count="40">
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -804,16 +798,9 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -830,13 +817,6 @@
         </right>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1235,15 +1215,15 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4BC5F24D-CAB9-4CFF-9A90-81F0A97CC23D}" name="Table2" displayName="Table2" ref="A1:F9" totalsRowShown="0" headerRowDxfId="7" dataDxfId="0" headerRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4BC5F24D-CAB9-4CFF-9A90-81F0A97CC23D}" name="Table2" displayName="Table2" ref="A1:F9" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7">
   <autoFilter ref="A1:F9" xr:uid="{B5EB7290-80D5-4166-A1AF-2F3EC711E8C0}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{C38A4344-5940-4D1A-954B-B327F67FC51B}" name="Citation" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{21871081-5263-4105-824F-702819BE3257}" name="Paper" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{5EC33F8F-E087-4F09-9973-DCEF253DE1F2}" name="Goals" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{8D925C0B-F22B-4B4B-9CB8-82AF34581EB3}" name="Used methods" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{149BEA12-A580-4BC7-8E8D-1A653C01B43F}" name="Results" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{B4C351CA-7B7B-4C23-A447-B3E32BD05355}" name="Why important (one sentence)" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{C38A4344-5940-4D1A-954B-B327F67FC51B}" name="Citation" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{21871081-5263-4105-824F-702819BE3257}" name="Paper" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{5EC33F8F-E087-4F09-9973-DCEF253DE1F2}" name="Goals" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{8D925C0B-F22B-4B4B-9CB8-82AF34581EB3}" name="Used methods" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{149BEA12-A580-4BC7-8E8D-1A653C01B43F}" name="Results" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{B4C351CA-7B7B-4C23-A447-B3E32BD05355}" name="Why important (one sentence)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1730,11 +1710,11 @@
       <c r="F2" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
     </row>
     <row r="3" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
@@ -1753,9 +1733,9 @@
       <c r="F3" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
     </row>
     <row r="4" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
@@ -1962,7 +1942,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2019,49 +1999,49 @@
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B4" s="14" t="s">
         <v>89</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>88</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="F6" s="5"/>
     </row>

</xml_diff>

<commit_message>
MA plan introduced simple stuff with graphframes added added final task description added papers related to constraint languages but summary of them is not yet finally ready
</commit_message>
<xml_diff>
--- a/papers/references.xlsx
+++ b/papers/references.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ansk\github\Master-s-thesis\papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A3F371-FF88-42E1-AED7-516250735053}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{998B67A4-C9A1-40CE-9FE7-8520B92DFFF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model-driven engineering" sheetId="1" r:id="rId1"/>
     <sheet name="Models and metamodels" sheetId="2" r:id="rId2"/>
     <sheet name="Multilevel models" sheetId="3" r:id="rId3"/>
     <sheet name="Models@runtime" sheetId="4" r:id="rId4"/>
+    <sheet name="Constraints" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="142">
   <si>
     <t>Citation</t>
   </si>
@@ -515,6 +516,273 @@
   </si>
   <si>
     <t>The classification of used models at runtime contains three categories. Namely, models can be categorized by the purpose of their use, the language by which they are constructed, and, finally, by the area they represent.</t>
+  </si>
+  <si>
+    <t>Cites</t>
+  </si>
+  <si>
+    <t>A Framework for Generating Query Language Code from OCL Invariants</t>
+  </si>
+  <si>
+    <t>A Graph Query Language for EMF Models</t>
+  </si>
+  <si>
+    <t>A Query-based Verification Tool for UML Class Diagrams with OCL Invariants</t>
+  </si>
+  <si>
+    <t>Adaptive Temporal Query Modeling</t>
+  </si>
+  <si>
+    <t>An overview of the deco system data model and query language; query processing and optimization</t>
+  </si>
+  <si>
+    <t>APQL A Process-Model Query Language</t>
+  </si>
+  <si>
+    <t>EMF-IncQuery An integrated development environment for live model queries</t>
+  </si>
+  <si>
+    <t>GraphFrames An Integrated API for Mixing Graph and Relational Queries</t>
+  </si>
+  <si>
+    <t>Incremental Evaluation of Model Queries over EMF Models</t>
+  </si>
+  <si>
+    <t>Object Constraint Language (OCL) a definitive guide</t>
+  </si>
+  <si>
+    <t>OCL2PSQL An OCL-to-SQL Code-Generator for Model</t>
+  </si>
+  <si>
+    <t>Query modeling for entity search based on terms, categories, and examples</t>
+  </si>
+  <si>
+    <t>Query Models</t>
+  </si>
+  <si>
+    <t>Translating OCL to Graph Patterns</t>
+  </si>
+  <si>
+    <t>Using UMLOCL Constraints for Relational Database Design</t>
+  </si>
+  <si>
+    <t>VMQL A generic visual model query language</t>
+  </si>
+  <si>
+    <t>"@article{heidenreich2007framework,
+  title={A framework for generating query language code from OCL invariants},
+  author={Heidenreich, Florian and Wende, Christian and Demuth, Birgit},
+  journal={Electronic Communications of the EASST},
+  volume={9},
+  year={2007}
+}"</t>
+  </si>
+  <si>
+    <t>"@inproceedings{bergmann2011graph,
+  title={A graph query language for EMF models},
+  author={Bergmann, G{\'a}bor and Ujhelyi, Zolt{\'a}n and R{\'a}th, Istv{\'a}n and Varr{\'o}, D{\'a}niel},
+  booktitle={International Conference on Theory and Practice of Model Transformations},
+  pages={167--182},
+  year={2011},
+  organization={Springer}
+}"</t>
+  </si>
+  <si>
+    <t>"@inproceedings{wu2022qmaxuse,
+  title={QMaxUSE: A Query-based Verification Tool for UML Class Diagrams with OCL Invariants},
+  author={Wu, Hao},
+  booktitle={International Conference on Fundamental Approaches to Software Engineering},
+  pages={310--317},
+  year={2022},
+  organization={Springer, Cham}
+}
+"</t>
+  </si>
+  <si>
+    <t>"@inproceedings{peetz2012adaptive,
+  title={Adaptive temporal query modeling},
+  author={Peetz, Maria-Hendrike and Meij, Edgar and Rijke, Maarten de and Weerkamp, Wouter},
+  booktitle={European Conference on Information Retrieval},
+  pages={455--458},
+  year={2012},
+  organization={Springer}
+}"</t>
+  </si>
+  <si>
+    <t>"@article{park2013overview,
+  title={An overview of the deco system: data model and query language; query processing and optimization},
+  author={Park, Hyunjung and Pang, Richard and Parameswaran, Aditya and Garcia-Molina, Hector and Polyzotis, Neoklis and Widom, Jennifer},
+  journal={ACM SIGMOD Record},
+  volume={41},
+  number={4},
+  pages={22--27},
+  year={2013},
+  publisher={ACM New York, NY, USA}
+}"</t>
+  </si>
+  <si>
+    <t>"@inproceedings{ter2013apql,
+  title={APQL: A process-model query language},
+  author={Ter Hofstede, Arthur HM and Ouyang, Chun and Rosa, Marcello La and Song, Liang and Wang, Jianmin and Polyvyanyy, Artem},
+  booktitle={Asia-Pacific Conference on Business Process Management},
+  pages={23--38},
+  year={2013},
+  organization={Springer}
+}"</t>
+  </si>
+  <si>
+    <t>"@article{ujhelyi2015emf,
+  title={EMF-IncQuery: An integrated development environment for live model queries},
+  author={Ujhelyi, Zolt{\'a}n and Bergmann, G{\'a}bor and Heged{\"u}s, {\'A}bel and Horv{\'a}th, {\'A}kos and Izs{\'o}, Benedek and R{\'a}th, Istv{\'a}n and Szatm{\'a}ri, Zolt{\'a}n and Varr{\'o}, D{\'a}niel},
+  journal={Science of Computer Programming},
+  volume={98},
+  pages={80--99},
+  year={2015},
+  publisher={Elsevier}
+}"</t>
+  </si>
+  <si>
+    <t>"@inproceedings{dave2016graphframes,
+  title={Graphframes: an integrated api for mixing graph and relational queries},
+  author={Dave, Ankur and Jindal, Alekh and Li, Li Erran and Xin, Reynold and Gonzalez, Joseph and Zaharia, Matei},
+  booktitle={Proceedings of the fourth international workshop on graph data management experiences and systems},
+  pages={1--8},
+  year={2016}
+}"</t>
+  </si>
+  <si>
+    <t>"@inproceedings{bergmann2010incremental,
+  title={Incremental evaluation of model queries over EMF models},
+  author={Bergmann, G{\'a}bor and Horv{\'a}th, {\'A}kos and R{\'a}th, Istv{\'a}n and Varr{\'o}, D{\'a}niel and Balogh, Andr{\'a}s and Balogh, Zolt{\'a}n and {\"O}kr{\"o}s, Andr{\'a}s},
+  booktitle={International conference on model driven engineering languages and systems},
+  pages={76--90},
+  year={2010},
+  organization={Springer}
+}"</t>
+  </si>
+  <si>
+    <t>"@inproceedings{cabot2012object,
+  title={Object constraint language (OCL): a definitive guide},
+  author={Cabot, Jordi and Gogolla, Martin},
+  booktitle={International school on formal methods for the design of computer, communication and software systems},
+  pages={58--90},
+  year={2012},
+  organization={Springer}
+}"</t>
+  </si>
+  <si>
+    <t>"@inproceedings{nguyen2019ocl2psql,
+  title={OCL2PSQL: an OCL-to-SQL code-generator for model-driven engineering},
+  author={Nguyen Phuoc Bao, Hoang and Clavel, Manuel},
+  booktitle={International Conference on Future Data and Security Engineering},
+  pages={185--203},
+  year={2019},
+  organization={Springer}
+}"</t>
+  </si>
+  <si>
+    <t>"@article{balog2011query,
+  title={Query modeling for entity search based on terms, categories, and examples},
+  author={Balog, Krisztian and Bron, Marc and De Rijke, Maarten},
+  journal={ACM Transactions on Information Systems (TOIS)},
+  volume={29},
+  number={4},
+  pages={1--31},
+  year={2011},
+  publisher={ACM New York, NY, USA}
+}"</t>
+  </si>
+  <si>
+    <t>"@inproceedings{stein2004query,
+  title={Query models},
+  author={Stein, Dominik and Hanenberg, Stefan and Unland, Rainer},
+  booktitle={International Conference on the Unified Modeling Language},
+  pages={98--112},
+  year={2004},
+  organization={Springer}
+}"</t>
+  </si>
+  <si>
+    <t>"@inproceedings{bergmann2014translating,
+  title={Translating OCL to graph patterns},
+  author={Bergmann, G{\'a}bor},
+  booktitle={International Conference on Model Driven Engineering Languages and Systems},
+  pages={670--686},
+  year={2014},
+  organization={Springer}
+}"</t>
+  </si>
+  <si>
+    <t>"@inproceedings{demuth1999using,
+  title={Using UML/OCL constraints for relational database design},
+  author={Demuth, Birgit and Hussmann, Heinrich},
+  booktitle={International Conference on the Unified Modeling Language},
+  pages={598--613},
+  year={1999},
+  organization={Springer}
+}"</t>
+  </si>
+  <si>
+    <t>"@inproceedings{storrle2009vmql,
+  title={VMQL: A generic visual model query language},
+  author={Storrle, Harald},
+  booktitle={2009 IEEE Symposium on Visual Languages and Human-Centric Computing (VL/HCC)},
+  pages={199--206},
+  year={2009},
+  organization={IEEE}
+}"</t>
+  </si>
+  <si>
+    <t>One of the most preferred ways to define a domain is to use a graphical language because it significantly reduces entry-level contrasted to textual languages where one first needs to grasp some basic syntax.  A well-known example of such a language is UML. Nevertheless, simplicity does not always imply expressiveness. Taking into account all the available functionality of UML, it is impossible to design a system in a comprehensive way. (my words)
+Initially, OCL emerged as a supporting tool for UML to mitigate its limitations in the detailed specification of a system. Gradually, its ability to define metamodel, model restrictions, and system requirements spread the usage of OCL, especially in the domain of MDE.
+The essential properties of OCL are that it is a typed and side-effects-free language []. The former means that all queries are always bound to the context within which a query is executed. The latter implies that a query execution does not modify query data (my words).
+OCL is able to define the following constraints:
+1) invariant restrictions defined at the class level that must be satisfied with every instantiation
+2) rules which every derived field should confront while being computed
+3) pre- and post-specifications which must be true before and, respectively, after some operation is computed
+4) query rules to traverse system data and return information back to a user
+OCL allows navigating through classes, their attributes, and their relations among them denoted by associations. Navigation within attributes results either in a concrete value or a collection depending on the type. In its turn, navigation within associations results as well either in a concrete class or a collection of classes depending on the multiplicity specified by a user.</t>
+  </si>
+  <si>
+    <t>Basic principles of OCL and why it is needed for defining a system</t>
+  </si>
+  <si>
+    <t>A complete overview of OCL</t>
+  </si>
+  <si>
+    <t>"@book{warmer2003object,
+  title={The object constraint language: getting your models ready for MDA},
+  author={Warmer, Jos B and Kleppe, Anneke G},
+  year={2003},
+  publisher={Addison-Wesley Professional}
+}"</t>
+  </si>
+  <si>
+    <t>The object constraint language: getting your models ready for MDA</t>
+  </si>
+  <si>
+    <t>Definition of a constraint</t>
+  </si>
+  <si>
+    <t>A constraint is defined as a restriction on one or more values of (part of) an object-oriented model or system. (no rephrasing)</t>
+  </si>
+  <si>
+    <t>What UML and OCL calls a constraint has been known in database technology for a long time under various names, for example integrity constraints [8], [18] [15], integrity rule [4], and consistency constraints [10]. We will use the term integrity constraint to refer to constraints in relational databases. In [8], types of integrity constraints are identified that are encountered frequently in database schemas: --&gt; for personal notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The usage of OCL is not limited to only restricting domains designed with UML. Several other applications of this declarative language exist in other areas. Thus, here authors attempt to enforce business rules directly into a database schema via the transformation of OCL rules into constraints in a relational database.
+What is a constraint? This guy defines it in the following way: "A constraint is defined as a restriction on one or more values of (part of) an object-oriented model or system". Hence, any constraint is bound to a modeled system whose attributes are valid if a constraint is fulfilled.
+As summarized here, constraints are compartmentalized by the following classifications:
+1) System view constraints. Invariant constraint represents a system in its static state, where a condition must adhere independent of the moment of system execution. Guard constraint represents a system in its dynamic state to check the permissibility of a transition from one state to another. 
+2) Constraint violation policy to specify an action in case of constraint failure.
+The latter category is crucial to consider if a model evolves and there is a high chance for a constraint infraction at some moment. For example, constraints can be further classified as advisable and primary. In case of violation, the latter would require human intervention to correct the state. Alternatively, the state of a model could also potentially be restored automatically.
+</t>
+  </si>
+  <si>
+    <t>It can be potentially used as related work</t>
+  </si>
+  <si>
+    <t>This approach has support for pattern matching and optimizations to boost performance</t>
   </si>
 </sst>
 </file>
@@ -645,7 +913,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -687,13 +955,61 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="49">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -1170,60 +1486,78 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8285077E-5915-4057-BA77-1D27902F310A}" name="Table1" displayName="Table1" ref="A1:F7" totalsRowShown="0" headerRowDxfId="39" dataDxfId="37" headerRowBorderDxfId="38" tableBorderDxfId="36" totalsRowBorderDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8285077E-5915-4057-BA77-1D27902F310A}" name="Table1" displayName="Table1" ref="A1:F7" totalsRowShown="0" headerRowDxfId="48" dataDxfId="46" headerRowBorderDxfId="47" tableBorderDxfId="45" totalsRowBorderDxfId="44">
   <autoFilter ref="A1:F7" xr:uid="{BA718EE1-49D7-4650-B037-0771614423BF}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{FF3B8A2A-F932-41FA-95FE-F39F73C1F2C4}" name="Citation" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{9B6745B4-27F0-426A-8DDC-565EB29CD89F}" name="Paper" dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{07897410-23B2-4D10-BE84-96D70F98FBC6}" name="Goals" dataDxfId="32"/>
-    <tableColumn id="6" xr3:uid="{A1146B1C-F33C-432E-90B6-E265AC99A77B}" name="Used methods" dataDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{04662BCC-AEE1-4C61-887F-F2AF7BAE3722}" name="Results" dataDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{0DF0A271-EB9F-4F3F-959F-4DECC9AAB759}" name="Why important (one sentence)" dataDxfId="29"/>
+    <tableColumn id="1" xr3:uid="{FF3B8A2A-F932-41FA-95FE-F39F73C1F2C4}" name="Citation" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{9B6745B4-27F0-426A-8DDC-565EB29CD89F}" name="Paper" dataDxfId="42"/>
+    <tableColumn id="5" xr3:uid="{07897410-23B2-4D10-BE84-96D70F98FBC6}" name="Goals" dataDxfId="41"/>
+    <tableColumn id="6" xr3:uid="{A1146B1C-F33C-432E-90B6-E265AC99A77B}" name="Used methods" dataDxfId="40"/>
+    <tableColumn id="3" xr3:uid="{04662BCC-AEE1-4C61-887F-F2AF7BAE3722}" name="Results" dataDxfId="39"/>
+    <tableColumn id="4" xr3:uid="{0DF0A271-EB9F-4F3F-959F-4DECC9AAB759}" name="Why important (one sentence)" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{822ADA59-34C7-4394-AE31-5D8AD6802D70}" name="Table3" displayName="Table3" ref="A1:F7" totalsRowShown="0" headerRowDxfId="28" dataDxfId="26" headerRowBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{822ADA59-34C7-4394-AE31-5D8AD6802D70}" name="Table3" displayName="Table3" ref="A1:F7" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36">
   <autoFilter ref="A1:F7" xr:uid="{DBC3082E-8AB2-4060-B752-8823303D327C}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{04A3358C-38AC-41A2-9EF8-F78CF5E86A8B}" name="Citation" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{07437842-31FC-44BC-A480-C79738F8C3E8}" name="Paper" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{C6E7F471-DA9B-4BD0-8B32-356D9F201A60}" name="Goals" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{FBBB0C1C-EB51-4A40-AA30-BEA588E8E954}" name="Used methods" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{B26D925F-D757-43CA-B039-C3186A8D2D00}" name="Results" dataDxfId="21"/>
-    <tableColumn id="6" xr3:uid="{19B8339E-AF8E-4C2D-9935-DF88EDB3038A}" name="Why important (one sentence)" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{04A3358C-38AC-41A2-9EF8-F78CF5E86A8B}" name="Citation" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{07437842-31FC-44BC-A480-C79738F8C3E8}" name="Paper" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{C6E7F471-DA9B-4BD0-8B32-356D9F201A60}" name="Goals" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{FBBB0C1C-EB51-4A40-AA30-BEA588E8E954}" name="Used methods" dataDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{B26D925F-D757-43CA-B039-C3186A8D2D00}" name="Results" dataDxfId="30"/>
+    <tableColumn id="6" xr3:uid="{19B8339E-AF8E-4C2D-9935-DF88EDB3038A}" name="Why important (one sentence)" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DFDAF967-C688-4C03-A27F-5FD297F6AB37}" name="Table4" displayName="Table4" ref="A7:F11" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16" totalsRowBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DFDAF967-C688-4C03-A27F-5FD297F6AB37}" name="Table4" displayName="Table4" ref="A7:F11" totalsRowShown="0" headerRowDxfId="28" dataDxfId="26" headerRowBorderDxfId="27" tableBorderDxfId="25" totalsRowBorderDxfId="24">
   <autoFilter ref="A7:F11" xr:uid="{5E47718A-97F9-432C-B83E-51A5A64721F9}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{42E1F1A7-0EDD-487C-B287-C83C32773D6F}" name="Citation" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{85E079A5-BC8D-4735-863E-AE69887C7784}" name="Paper" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{1998B378-71BB-42A6-BD3B-B6DB7CF49B9F}" name="Goals" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{E40C5699-D930-4E6B-80D1-80A1E126EA5E}" name="Used methods" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{E32B528D-F116-49F3-9313-33D9BB463AAC}" name="Results" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{7AA69EB9-56A4-470C-B997-C9AF00351BC6}" name="Why important (one sentence)" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{42E1F1A7-0EDD-487C-B287-C83C32773D6F}" name="Citation" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{85E079A5-BC8D-4735-863E-AE69887C7784}" name="Paper" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{1998B378-71BB-42A6-BD3B-B6DB7CF49B9F}" name="Goals" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{E40C5699-D930-4E6B-80D1-80A1E126EA5E}" name="Used methods" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{E32B528D-F116-49F3-9313-33D9BB463AAC}" name="Results" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{7AA69EB9-56A4-470C-B997-C9AF00351BC6}" name="Why important (one sentence)" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4BC5F24D-CAB9-4CFF-9A90-81F0A97CC23D}" name="Table2" displayName="Table2" ref="A1:F9" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4BC5F24D-CAB9-4CFF-9A90-81F0A97CC23D}" name="Table2" displayName="Table2" ref="A1:F9" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16">
   <autoFilter ref="A1:F9" xr:uid="{B5EB7290-80D5-4166-A1AF-2F3EC711E8C0}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{C38A4344-5940-4D1A-954B-B327F67FC51B}" name="Citation" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{21871081-5263-4105-824F-702819BE3257}" name="Paper" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{5EC33F8F-E087-4F09-9973-DCEF253DE1F2}" name="Goals" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{8D925C0B-F22B-4B4B-9CB8-82AF34581EB3}" name="Used methods" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{149BEA12-A580-4BC7-8E8D-1A653C01B43F}" name="Results" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{B4C351CA-7B7B-4C23-A447-B3E32BD05355}" name="Why important (one sentence)" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{C38A4344-5940-4D1A-954B-B327F67FC51B}" name="Citation" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{21871081-5263-4105-824F-702819BE3257}" name="Paper" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{5EC33F8F-E087-4F09-9973-DCEF253DE1F2}" name="Goals" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{8D925C0B-F22B-4B4B-9CB8-82AF34581EB3}" name="Used methods" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{149BEA12-A580-4BC7-8E8D-1A653C01B43F}" name="Results" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{B4C351CA-7B7B-4C23-A447-B3E32BD05355}" name="Why important (one sentence)" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{CB7E7626-1A07-4A63-A1BB-45411799C9DB}" name="Table5" displayName="Table5" ref="A1:F29" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7">
+  <autoFilter ref="A1:F29" xr:uid="{AACD61C1-93F4-4A91-BF1C-525D28CD130A}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F29">
+    <sortCondition descending="1" ref="C1:C29"/>
+  </sortState>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{59DD8826-9FE0-43E3-92E9-676A847412AA}" name="Citation" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{64695F29-51F8-44DE-B0D3-A6297CA3B3A2}" name="Paper" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{130E129D-E582-479C-A728-F0E15CADF9D7}" name="Cites" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{B1D8EA51-E674-4514-89D2-25E93017739C}" name="Goals" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{FE122979-06A9-4524-9891-A13CE2BE6292}" name="Results" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{501FD3AA-E18D-4F75-A575-94FB96D18379}" name="Why important (one sentence)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1710,11 +2044,11 @@
       <c r="F2" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
     </row>
     <row r="3" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
@@ -1733,9 +2067,9 @@
       <c r="F3" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
     </row>
     <row r="4" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
@@ -1941,8 +2275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C75DB7F1-B501-46CE-AB52-85AC9D327FEE}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2075,4 +2409,395 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{909D06DD-0136-4BF5-A323-796F63E6F11F}">
+  <dimension ref="A1:F29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.77734375" customWidth="1"/>
+    <col min="2" max="2" width="42.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.109375" customWidth="1"/>
+    <col min="5" max="5" width="80.88671875" customWidth="1"/>
+    <col min="6" max="6" width="33.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" s="14">
+        <v>1437</v>
+      </c>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="14">
+        <v>229</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" s="15">
+        <v>168</v>
+      </c>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+    </row>
+    <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" s="14">
+        <v>153</v>
+      </c>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="15">
+        <v>131</v>
+      </c>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+    </row>
+    <row r="7" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="14">
+        <v>109</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="C8" s="14">
+        <v>106</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+    </row>
+    <row r="9" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" s="14">
+        <v>98</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+    </row>
+    <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="C10" s="14">
+        <v>79</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+    </row>
+    <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="C11" s="14">
+        <v>60</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+    </row>
+    <row r="12" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12" s="14">
+        <v>47</v>
+      </c>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+    </row>
+    <row r="13" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C13" s="14">
+        <v>46</v>
+      </c>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+    </row>
+    <row r="14" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C14" s="14">
+        <v>42</v>
+      </c>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+    </row>
+    <row r="15" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="C15" s="14">
+        <v>29</v>
+      </c>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+    </row>
+    <row r="16" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="C16" s="14">
+        <v>20</v>
+      </c>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+    </row>
+    <row r="17" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17" s="14">
+        <v>8</v>
+      </c>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+    </row>
+    <row r="18" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C18" s="14">
+        <v>1</v>
+      </c>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+    </row>
+    <row r="19" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+    </row>
+    <row r="20" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+    </row>
+    <row r="21" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="14"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+    </row>
+    <row r="22" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="14"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+    </row>
+    <row r="23" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="14"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+    </row>
+    <row r="24" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+    </row>
+    <row r="25" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="14"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+    </row>
+    <row r="26" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="14"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+    </row>
+    <row r="27" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="14"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+    </row>
+    <row r="28" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="14"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+    </row>
+    <row r="29" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="14"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Working on constraints languages subchapter, noted gremlin as related work
</commit_message>
<xml_diff>
--- a/papers/references.xlsx
+++ b/papers/references.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ansk\github\Master-s-thesis\papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{998B67A4-C9A1-40CE-9FE7-8520B92DFFF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5319D54C-8544-438E-839F-EBFBFBBE3396}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,6 +20,7 @@
     <sheet name="Constraints" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="160">
   <si>
     <t>Citation</t>
   </si>
@@ -527,18 +528,6 @@
     <t>A Graph Query Language for EMF Models</t>
   </si>
   <si>
-    <t>A Query-based Verification Tool for UML Class Diagrams with OCL Invariants</t>
-  </si>
-  <si>
-    <t>Adaptive Temporal Query Modeling</t>
-  </si>
-  <si>
-    <t>An overview of the deco system data model and query language; query processing and optimization</t>
-  </si>
-  <si>
-    <t>APQL A Process-Model Query Language</t>
-  </si>
-  <si>
     <t>EMF-IncQuery An integrated development environment for live model queries</t>
   </si>
   <si>
@@ -549,12 +538,6 @@
   </si>
   <si>
     <t>Object Constraint Language (OCL) a definitive guide</t>
-  </si>
-  <si>
-    <t>OCL2PSQL An OCL-to-SQL Code-Generator for Model</t>
-  </si>
-  <si>
-    <t>Query modeling for entity search based on terms, categories, and examples</t>
   </si>
   <si>
     <t>Query Models</t>
@@ -584,49 +567,6 @@
   booktitle={International Conference on Theory and Practice of Model Transformations},
   pages={167--182},
   year={2011},
-  organization={Springer}
-}"</t>
-  </si>
-  <si>
-    <t>"@inproceedings{wu2022qmaxuse,
-  title={QMaxUSE: A Query-based Verification Tool for UML Class Diagrams with OCL Invariants},
-  author={Wu, Hao},
-  booktitle={International Conference on Fundamental Approaches to Software Engineering},
-  pages={310--317},
-  year={2022},
-  organization={Springer, Cham}
-}
-"</t>
-  </si>
-  <si>
-    <t>"@inproceedings{peetz2012adaptive,
-  title={Adaptive temporal query modeling},
-  author={Peetz, Maria-Hendrike and Meij, Edgar and Rijke, Maarten de and Weerkamp, Wouter},
-  booktitle={European Conference on Information Retrieval},
-  pages={455--458},
-  year={2012},
-  organization={Springer}
-}"</t>
-  </si>
-  <si>
-    <t>"@article{park2013overview,
-  title={An overview of the deco system: data model and query language; query processing and optimization},
-  author={Park, Hyunjung and Pang, Richard and Parameswaran, Aditya and Garcia-Molina, Hector and Polyzotis, Neoklis and Widom, Jennifer},
-  journal={ACM SIGMOD Record},
-  volume={41},
-  number={4},
-  pages={22--27},
-  year={2013},
-  publisher={ACM New York, NY, USA}
-}"</t>
-  </si>
-  <si>
-    <t>"@inproceedings{ter2013apql,
-  title={APQL: A process-model query language},
-  author={Ter Hofstede, Arthur HM and Ouyang, Chun and Rosa, Marcello La and Song, Liang and Wang, Jianmin and Polyvyanyy, Artem},
-  booktitle={Asia-Pacific Conference on Business Process Management},
-  pages={23--38},
-  year={2013},
   organization={Springer}
 }"</t>
   </si>
@@ -668,28 +608,6 @@
   pages={58--90},
   year={2012},
   organization={Springer}
-}"</t>
-  </si>
-  <si>
-    <t>"@inproceedings{nguyen2019ocl2psql,
-  title={OCL2PSQL: an OCL-to-SQL code-generator for model-driven engineering},
-  author={Nguyen Phuoc Bao, Hoang and Clavel, Manuel},
-  booktitle={International Conference on Future Data and Security Engineering},
-  pages={185--203},
-  year={2019},
-  organization={Springer}
-}"</t>
-  </si>
-  <si>
-    <t>"@article{balog2011query,
-  title={Query modeling for entity search based on terms, categories, and examples},
-  author={Balog, Krisztian and Bron, Marc and De Rijke, Maarten},
-  journal={ACM Transactions on Information Systems (TOIS)},
-  volume={29},
-  number={4},
-  pages={1--31},
-  year={2011},
-  publisher={ACM New York, NY, USA}
 }"</t>
   </si>
   <si>
@@ -779,10 +697,133 @@
 </t>
   </si>
   <si>
-    <t>It can be potentially used as related work</t>
-  </si>
-  <si>
     <t>This approach has support for pattern matching and optimizations to boost performance</t>
+  </si>
+  <si>
+    <t>About constraints: https://neo4j.com/docs/cypher-manual/4.4/constraints/</t>
+  </si>
+  <si>
+    <t>Germlin -&gt;tinkerpop</t>
+  </si>
+  <si>
+    <t>Epsilon</t>
+  </si>
+  <si>
+    <t>This paper is related to Viatra (part of related work), has table 4 as comparison of query languages; also talk a lot about "incremental query evaluation" that is stated to boost the performance</t>
+  </si>
+  <si>
+    <t>Model queries are important components in model-driven tool chains. They are widely used in model transformations, model execution/simulation, report generation, or the evaluation of well-formedness constraints.
+In current industrial applications based on popular modeling frameworks (e.g. the Eclipse Modeling Framework EMF[1]), model queries are still frequently implemented using a traditional programming language (Java), despite the availability of more advanced declarative query languages such as OCL [2] or EMF Model Query [3]. The reasons for this are two-fold. Unfortunately, as observed in tool development practice, as well as in benchmark measurements [4], the implementation infrastructure behind these high level model query languages often has scalability issues when large instance models are used, which may effectively rule out the application of these technologies in certain industrial applications. Additional issues include expressiveness and learning effort. Simple technologies (such as EMF Model Query) are not flexible or expressive enough for advanced use cases involving complex join operations, while complex – and thus significantly harder to learn [5] – languages such as OCL still lack important features despite their higher expressive power. Such important features include reusable query modularization, recursion and transitive closures, which are not easily accessible or not supported at all. Finally, there is also a practical need for the adaptation and extension of compile-time validation techniques, which are currently in very early stages of development.
+In [4], we demonstrated how incremental model transformation techniques of the Viatra2 framework can be adapted to efficiently support advanced model queries over large EMF models and proposed a new runtime model query framework called EMF-IncQuery. Our initial investigations were focused on providing high performance for model queries, therefore, we reused the query language of Viatra2. However, as the underlying (meta-)modeling foundations for Viatra2 and EMF are different, the direct reuse of the Viatra2 graph pattern language raised usability issues.</t>
+  </si>
+  <si>
+    <t>NOT ADAPTED!</t>
+  </si>
+  <si>
+    <t>Interesting paper about transforming ocl statements to other query languages like SQL. Done in two stages: 1) schema transformation 2) constraint transformation</t>
+  </si>
+  <si>
+    <t>nothing to be quoted so far</t>
+  </si>
+  <si>
+    <t>specification of queries is a new emerging design issue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Join Point Designation Diagrams
+IDEA -&gt; PROVIDE EXAMPLE OF SOME COMPLEX QUERIES IN RELATED WORK CONDLUSION TO STATE THAT USER NEEDS A UI AND LINK WITH THIS WORK. As a conclusion from the previous investigations, we attest textual notations to leave developers stranded with a heavy load of complexity: Developers are required to have a profound understanding about the usage of keywords and operators in order to specify queries properly. They must know what properties of what elements they may refer to, and how. Finally, they must have high analytical capabilities in order to assess the grouping of selection criteria as well as their semantic interdependencies, so that they can estimate what elements will be actually retrieved. Opposed to so much complexity, developers urgently call for a graphical notation that help them with the composition and comprehension of selection queries. That notation should give them a visual conception of the selection semantics they are currently specifying using textual keywords. It should facilitate the specification of selection criteria on elements and their properties. Furthermore, it should depict the grouping of such selection criteria and visualize their interdependencies. In order to come up with more concrete characteristics that our graphical notation must possess, we revisit the examples of the previous sections and investigate what different kinds of selections we have used: First of all, we may observe that – even though each notation comes with its own, most individual syntax, keywords, and operators – they are all concerned with the selection of (more or less) the same program elements, namely classes and objects, as well as the relationships between them (i.e., association relationships, generalization relationships, and call dependencies). Further, we recognize that selection is almost always based on the element names (only sometimes the elements name does not matter). Apart from that, selection may be based on the element's structural composition; for example, based on the (non-)existence of features in classes or of parameters in a parameter list. The last observation we make is that selection of elements is often based on the general context they reside in; meaning that query specifications abstract from (a set of) direct relationships between elements and merely call for the existence of paths. </t>
+  </si>
+  <si>
+    <t>about how to query models in MDA, introduced UI and engine to query models</t>
+  </si>
+  <si>
+    <t>Related to Viatra again. Transform ocl to graph for querying. Provide nice performance comparison</t>
+  </si>
+  <si>
+    <t>Viatra?</t>
+  </si>
+  <si>
+    <t>GOAL: The current paper presents an automatic mapping from a large sublanguage of OCL expressions to equivalent graph patterns in the dialect of EMF-IncQuery. Validation of benefits is carried out by performance measurements according to an existing benchmark
+Model-driven tools use model queries for many purposes, including validation of well-formedness rules and specification of derived features. The majority of declarative model query corpus available in industry appears to use the OCL language. Graph pattern based queries, however, would have a number of advantages due to their more abstract specification, such as performance improvements through advanced query evaluation techniques. As query performance can be a key issue with large models, evaluating graph patterns instead of OCL queries could be useful in practice</t>
+  </si>
+  <si>
+    <t>Imperative vs. Declarative Query Languages: What’s the Difference? - SEPARATE SUBCHAPTER??</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Predefined queries (PDQ) -&gt; to predefined constraints?? </t>
+  </si>
+  <si>
+    <t>Both of these disadvantages are avoided by Constraint Diagrams [4]. Here, the concrete syntax (which is much less likely to change than the meta-model) is used to formulate a query. Unfortunately, Constraint Diagrams are rather limited with respect to the modeling language they may be applied to (basic class diagrams). Also, it seems that Constraint Diagrams have never been implemented as a tool.</t>
+  </si>
+  <si>
+    <t>User-driven query system for modelling mde artifacts</t>
+  </si>
+  <si>
+    <t>It will be used as related work</t>
+  </si>
+  <si>
+    <t>DYNAMIC CONSTRAINTS OR CONSTRAINTS AT RUNTIME</t>
+  </si>
+  <si>
+    <t>"@inproceedings{silva1997dynamic,
+  title={Dynamic integrity constraints definition and enforcement in databases: a classification framework},
+  author={Silva, MA},
+  booktitle={Working Conference on Integrity and Internal Control in Information Systems},
+  pages={65--87},
+  year={1997},
+  organization={Springer}
+}"</t>
+  </si>
+  <si>
+    <t>Dynamic integrity constraints definition and enforcement in databases: a classification framework</t>
+  </si>
+  <si>
+    <t>Database communities emphasize dynamic constraints to formulate conditions over multiple entity states to enforce integrity consistency of the schema during its evolution.</t>
+  </si>
+  <si>
+    <t>Evolution in dynamic software product lines: challenges and perspectives</t>
+  </si>
+  <si>
+    <t>"@inproceedings{quinton2015evolution,
+  title={Evolution in dynamic software product lines: challenges and perspectives},
+  author={Quinton, Cl{\'e}ment and Rabiser, Rick and Vierhauser, Michael and Gr{\"u}nbacher, Paul and Baresi, Luciano},
+  booktitle={Proceedings of the 19th International Conference on Software Product Line},
+  pages={126--130},
+  year={2015}
+}"</t>
+  </si>
+  <si>
+    <t>"@inproceedings{dinkelaker2010dynamic,
+  title={A dynamic software product line approach using aspect models at runtime},
+  author={Dinkelaker, Tom and Mitschke, Ralf and Fetzer, Karin and Mezini, Mira},
+  booktitle={5th Domain-Specific Aspect Languages Workshop},
+  year={2010}
+}"</t>
+  </si>
+  <si>
+    <t>A Dynamic Software Product Line Approach using Aspect Models at Runtime</t>
+  </si>
+  <si>
+    <t>Towards a Model-Integrated Runtime Monitoring Infrastructure for Cyber-Physical Systems</t>
+  </si>
+  <si>
+    <t>"@inproceedings{vierhauser2021towards,
+  title={Towards a model-integrated runtime monitoring infrastructure for cyber-physical systems},
+  author={Vierhauser, Michael and Marah, Hussein and Garmendia, Antonio and Cleland-Huang, Jane and Wimmer, Manuel},
+  booktitle={2021 IEEE/ACM 43rd International Conference on Software Engineering: New Ideas and Emerging Results (ICSE-NIER)},
+  pages={96--100},
+  year={2021},
+  organization={IEEE}
+}"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Library-Based Appr y-Based Approach to Translating OCL Constr anslating OCL Constraints t aints to JML Assertions for Runtime Checking </t>
+  </si>
+  <si>
+    <t>"@article{avila2008library,
+  title={A library-based approach to translating OCL constraints to JML assertions for runtime checking},
+  author={Avila, Carmen and Flores Jr, Guillermo and Cheon, Yoonsik},
+  year={2008}
+}"</t>
   </si>
 </sst>
 </file>
@@ -913,7 +954,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -961,6 +1002,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1546,10 +1590,10 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{CB7E7626-1A07-4A63-A1BB-45411799C9DB}" name="Table5" displayName="Table5" ref="A1:F29" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7">
-  <autoFilter ref="A1:F29" xr:uid="{AACD61C1-93F4-4A91-BF1C-525D28CD130A}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F29">
-    <sortCondition descending="1" ref="C1:C29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{CB7E7626-1A07-4A63-A1BB-45411799C9DB}" name="Table5" displayName="Table5" ref="A1:F23" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7">
+  <autoFilter ref="A1:F23" xr:uid="{AACD61C1-93F4-4A91-BF1C-525D28CD130A}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F23">
+    <sortCondition ref="E1:E23"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{59DD8826-9FE0-43E3-92E9-676A847412AA}" name="Citation" dataDxfId="5"/>
@@ -1842,7 +1886,7 @@
     <col min="6" max="6" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2044,11 +2088,11 @@
       <c r="F2" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
     </row>
     <row r="3" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
@@ -2067,9 +2111,9 @@
       <c r="F3" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
     </row>
     <row r="4" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
@@ -2289,7 +2333,7 @@
     <col min="6" max="6" width="36.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2413,10 +2457,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{909D06DD-0136-4BF5-A323-796F63E6F11F}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2429,7 +2473,7 @@
     <col min="6" max="6" width="33.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2449,258 +2493,296 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="C2" s="14">
         <v>1437</v>
       </c>
       <c r="D2" s="14"/>
       <c r="E2" s="14" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+      <c r="H2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>108</v>
       </c>
       <c r="C3" s="14">
-        <v>229</v>
+        <v>20</v>
       </c>
       <c r="D3" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="H3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" s="14">
+        <v>47</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="H4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5" s="14">
+        <v>60</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="H5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="14">
+        <v>98</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="E6" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="F3" s="14" t="s">
+      <c r="F6" s="14" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="C4" s="15">
-        <v>168</v>
-      </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-    </row>
-    <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="C5" s="14">
-        <v>153</v>
-      </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="C6" s="15">
-        <v>131</v>
-      </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-    </row>
-    <row r="7" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C7" s="14">
-        <v>109</v>
+        <v>79</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="H7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" s="14">
+        <v>229</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="H8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" s="14">
+        <v>153</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="C10" s="14">
+        <v>109</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" s="15">
+        <v>168</v>
+      </c>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="F7" s="14" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="C8" s="14">
-        <v>106</v>
-      </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-    </row>
-    <row r="9" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="C9" s="14">
-        <v>98</v>
-      </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-    </row>
-    <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="C10" s="14">
-        <v>79</v>
-      </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-    </row>
-    <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="C11" s="14">
-        <v>60</v>
-      </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-    </row>
-    <row r="12" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="C12" s="14">
-        <v>47</v>
-      </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-    </row>
-    <row r="13" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="14" t="s">
-        <v>120</v>
-      </c>
+    </row>
+    <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" s="15">
+        <v>131</v>
+      </c>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="17" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="14"/>
       <c r="B13" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="C13" s="14">
-        <v>46</v>
-      </c>
+        <v>148</v>
+      </c>
+      <c r="C13" s="14"/>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
     </row>
-    <row r="14" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
-        <v>119</v>
+        <v>149</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="C14" s="14">
-        <v>42</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="C14" s="14"/>
       <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
+      <c r="E14" s="14" t="s">
+        <v>151</v>
+      </c>
       <c r="F14" s="14"/>
     </row>
-    <row r="15" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
-        <v>118</v>
+        <v>153</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="C15" s="14">
-        <v>29</v>
-      </c>
+        <v>152</v>
+      </c>
+      <c r="C15" s="14"/>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
       <c r="F15" s="14"/>
     </row>
-    <row r="16" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
-        <v>130</v>
+        <v>154</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="C16" s="14">
-        <v>20</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="C16" s="14"/>
       <c r="D16" s="14"/>
       <c r="E16" s="14"/>
       <c r="F16" s="14"/>
     </row>
     <row r="17" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
-        <v>125</v>
+        <v>157</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="C17" s="14">
-        <v>8</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="C17" s="14"/>
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
       <c r="F17" s="14"/>
     </row>
     <row r="18" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="s">
-        <v>117</v>
+        <v>159</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="C18" s="14">
-        <v>1</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="C18" s="14"/>
       <c r="D18" s="14"/>
       <c r="E18" s="14"/>
       <c r="F18" s="14"/>
@@ -2744,54 +2826,6 @@
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
       <c r="F23" s="14"/>
-    </row>
-    <row r="24" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="14"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-    </row>
-    <row r="25" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="14"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-    </row>
-    <row r="26" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="14"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-    </row>
-    <row r="27" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="14"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-    </row>
-    <row r="28" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="14"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-    </row>
-    <row r="29" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="14"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update MA PLAN.txt, A Graphical Query Language VISUAL and Its Query Processing.pdf, and 9 more files...
</commit_message>
<xml_diff>
--- a/papers/references.xlsx
+++ b/papers/references.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ansk\github\Master-s-thesis\papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5319D54C-8544-438E-839F-EBFBFBBE3396}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{761AF74C-F3F3-47B4-AA88-E8214570283F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,6 @@
     <sheet name="Constraints" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="163">
   <si>
     <t>Citation</t>
   </si>
@@ -824,6 +823,16 @@
   author={Avila, Carmen and Flores Jr, Guillermo and Cheon, Yoonsik},
   year={2008}
 }"</t>
+  </si>
+  <si>
+    <t>OCL as a language to declare constraints during design time is not able to validate constraints at runtime. Therefore, the violation of constraints cannot be detected during the system evolution. One needs another type of constraint that is sound in the presence of constant changes in the software and is able to adapt accordingly.</t>
+  </si>
+  <si>
+    <t>To prevent potential deviations at runtime a bound model to a running system must be restricted by constraints. Information regarding the abnormal behavior of a system should be delivered to an end-user through notification or report components that illustrate the up-to-date system data.
+However, just defining constraints in dynamic cyber-physical systems is not enough. The reason is that the initially defined constraints age and become outdated during the evolution of a system. Therefore, to provide correctness and soundness of the constraint analysis, the constraints should co-evolve together with the system. Neglecting the dynamic nature of constraints in such systems might lead to false-positive validation results or a lack of validity constraints in a runtime system.</t>
+  </si>
+  <si>
+    <t>INTUITIVE UI FOR QUERY</t>
   </si>
 </sst>
 </file>
@@ -2459,8 +2468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{909D06DD-0136-4BF5-A323-796F63E6F11F}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2739,29 +2748,29 @@
       </c>
       <c r="F14" s="14"/>
     </row>
-    <row r="15" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="14" t="s">
+    <row r="15" spans="1:8" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-    </row>
-    <row r="16" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="14" t="s">
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+    </row>
+    <row r="16" spans="1:8" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
     </row>
     <row r="17" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
@@ -2770,9 +2779,11 @@
       <c r="B17" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="C17" s="14"/>
+      <c r="C17" s="15"/>
       <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
+      <c r="E17" s="14" t="s">
+        <v>161</v>
+      </c>
       <c r="F17" s="14"/>
     </row>
     <row r="18" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -2784,12 +2795,16 @@
       </c>
       <c r="C18" s="14"/>
       <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
+      <c r="E18" s="14" t="s">
+        <v>160</v>
+      </c>
       <c r="F18" s="14"/>
     </row>
     <row r="19" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
-      <c r="B19" s="14"/>
+      <c r="B19" s="14" t="s">
+        <v>162</v>
+      </c>
       <c r="C19" s="14"/>
       <c r="D19" s="14"/>
       <c r="E19" s="14"/>

</xml_diff>

<commit_message>
Intuitive ui part is almost ready, parts about constraint languages in general are not yet adopted
</commit_message>
<xml_diff>
--- a/papers/references.xlsx
+++ b/papers/references.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ansk\github\Master-s-thesis\papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{761AF74C-F3F3-47B4-AA88-E8214570283F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF2792A-53A4-4891-A9C0-29186FAFB6DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model-driven engineering" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="171">
   <si>
     <t>Citation</t>
   </si>
@@ -834,12 +834,48 @@
   <si>
     <t>INTUITIVE UI FOR QUERY</t>
   </si>
+  <si>
+    <t>QUERY DATA VS CONSTRAINT DATA (ALL MY OWN WORDS)
+Even though the primary focus of this work is finding ways of effectively restricting runtime models, this section will provide a foundation narrative of visual query languages.
+To shed the light on the difference (if such even exists) between data constraints and query constraints let us consider the following example.
+Suppose to have a small application that manages delivery service for a local restaurant. Usually, administration staff makes sure that more than one delivery guy is available at shift. The minimal requirement, however, is to have at least one member that delivers orders.
+This constraint could be described via a well-known OCL like this. On the other hand, the same result is achieved by writing a query in SQL.
+Therefore, calling something a constraint means shaping what your data should or should not look like. Meanwhile, the query describes a pattern match to satisfy defined properties. Since they both serve the same objective any constraint can also be expressed by a query.</t>
+  </si>
+  <si>
+    <t>GoRelations An Intuitive Query System for Dbpedia</t>
+  </si>
+  <si>
+    <t>Natural language systems are a perfect candidate to lower the high entry level for building queries by end-users. This is because such systems can synthesize a legit query from a simple text understandable for any human being.</t>
+  </si>
+  <si>
+    <t>How Useful Are Natural Language Interfaces to the Semantic Web for Casual End-Users?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">While being an intuitive tool for an end-user that hides the complexity of query syntax, multiple issues make the design and implementation of a natural language for a query language non-trivial and time-demanding. Those limitations are summarized in the work of the author and mentioned below:
+1) the performance of a natural query language is correlated with its closeness to the domain. The closer it is bound to a specific domain, the deeper the semantic can be exploited by this.
+2) however, a natural query language that is tied to a particular domain spoils its adaptability
+3) natural query languages are rich in expressiveness, which implies their ambiguity by their nature. 
+Even though some ideas to overcome some of the limitations mentioned above are presented in work, the fact that a natural query language is tightened with context makes it inconceivable to reuse in other domains. </t>
+  </si>
+  <si>
+    <t>NITELIGHT: A Graphical Tool for Semantic Query Construction</t>
+  </si>
+  <si>
+    <t>As opposed to natural query languages, one could offer an environment with an interactive graphical interface to build queries. Visual query systems aim at providing means for visual query specification. As summarized in the work of [], we should consider three types of interfaces for visual query construction.
+1) icon-based interface. It offers a query construction by utilizing icons supplemented by meta query information to specify queries without the need to access actual data. One of the systems that use such an interface is VISION (reference)
+2) form-based interface. It offers a set of structured components. Users only have to fill out predefined forms by the required criteria, and a query will be constructed automatically by a respective software vendor. Perhaps, one of the most famous examples of this category is the "Query By Example" system (reference)
+3) diagram-based interface. It depicts a query construction using some geometrical figures presenting entities, often with connectors representing relations between them.</t>
+  </si>
+  <si>
+    <t>KalNdoquery: A Visual Query Language for Object Databases</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -853,6 +889,15 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -963,7 +1008,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1016,6 +1061,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1885,17 +1933,17 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.21875" customWidth="1"/>
-    <col min="2" max="2" width="26.5546875" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
-    <col min="5" max="5" width="64.44140625" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="64.42578125" customWidth="1"/>
     <col min="6" max="6" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1915,7 +1963,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -1935,7 +1983,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1955,7 +2003,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>6</v>
       </c>
@@ -1975,7 +2023,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -1995,7 +2043,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
@@ -2015,7 +2063,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="225" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>19</v>
       </c>
@@ -2052,17 +2100,17 @@
       <selection activeCell="F1" sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" customWidth="1"/>
-    <col min="4" max="4" width="15.77734375" customWidth="1"/>
-    <col min="5" max="5" width="67.77734375" customWidth="1"/>
-    <col min="6" max="6" width="27.5546875" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="67.7109375" customWidth="1"/>
+    <col min="6" max="6" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2082,7 +2130,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>50</v>
       </c>
@@ -2103,7 +2151,7 @@
       <c r="I2" s="18"/>
       <c r="J2" s="18"/>
     </row>
-    <row r="3" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>41</v>
       </c>
@@ -2124,7 +2172,7 @@
       <c r="I3" s="18"/>
       <c r="J3" s="18"/>
     </row>
-    <row r="4" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>62</v>
       </c>
@@ -2138,7 +2186,7 @@
       </c>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>58</v>
       </c>
@@ -2154,7 +2202,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="331.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="390" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>43</v>
       </c>
@@ -2174,7 +2222,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="331.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="360" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>64</v>
       </c>
@@ -2207,42 +2255,42 @@
       <selection activeCell="A7" sqref="A7:F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5546875" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" customWidth="1"/>
-    <col min="5" max="5" width="66.6640625" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="66.7109375" customWidth="1"/>
     <col min="6" max="6" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -2262,7 +2310,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>76</v>
       </c>
@@ -2278,7 +2326,7 @@
       </c>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:6" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>77</v>
       </c>
@@ -2290,7 +2338,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>78</v>
       </c>
@@ -2304,7 +2352,7 @@
       </c>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>79</v>
       </c>
@@ -2332,17 +2380,17 @@
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" customWidth="1"/>
-    <col min="2" max="2" width="18.77734375" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="15.21875" customWidth="1"/>
-    <col min="5" max="5" width="71.88671875" customWidth="1"/>
-    <col min="6" max="6" width="36.21875" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="71.85546875" customWidth="1"/>
+    <col min="6" max="6" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2362,7 +2410,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>84</v>
       </c>
@@ -2376,7 +2424,7 @@
       </c>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:6" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>87</v>
       </c>
@@ -2390,7 +2438,7 @@
       </c>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:6" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>89</v>
       </c>
@@ -2404,7 +2452,7 @@
       </c>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>91</v>
       </c>
@@ -2418,7 +2466,7 @@
       </c>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>93</v>
       </c>
@@ -2432,7 +2480,7 @@
       </c>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -2440,7 +2488,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -2448,7 +2496,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -2468,21 +2516,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{909D06DD-0136-4BF5-A323-796F63E6F11F}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.77734375" customWidth="1"/>
-    <col min="2" max="2" width="42.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.109375" customWidth="1"/>
-    <col min="5" max="5" width="80.88671875" customWidth="1"/>
-    <col min="6" max="6" width="33.109375" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" customWidth="1"/>
+    <col min="5" max="5" width="80.85546875" customWidth="1"/>
+    <col min="6" max="6" width="33.140625" customWidth="1"/>
+    <col min="8" max="8" width="150.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2502,7 +2551,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>122</v>
       </c>
@@ -2523,7 +2572,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>118</v>
       </c>
@@ -2546,7 +2595,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>116</v>
       </c>
@@ -2569,7 +2618,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>115</v>
       </c>
@@ -2592,7 +2641,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>110</v>
       </c>
@@ -2612,7 +2661,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>109</v>
       </c>
@@ -2633,7 +2682,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>114</v>
       </c>
@@ -2656,7 +2705,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>117</v>
       </c>
@@ -2674,7 +2723,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>112</v>
       </c>
@@ -2692,7 +2741,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>111</v>
       </c>
@@ -2707,8 +2756,11 @@
       <c r="F11" s="17" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H11" s="19" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>113</v>
       </c>
@@ -2724,9 +2776,9 @@
         <v>141</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="19" t="s">
         <v>148</v>
       </c>
       <c r="C13" s="14"/>
@@ -2734,7 +2786,7 @@
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
     </row>
-    <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>149</v>
       </c>
@@ -2748,7 +2800,7 @@
       </c>
       <c r="F14" s="14"/>
     </row>
-    <row r="15" spans="1:8" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>153</v>
       </c>
@@ -2760,7 +2812,7 @@
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
     </row>
-    <row r="16" spans="1:8" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>154</v>
       </c>
@@ -2772,7 +2824,7 @@
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
     </row>
-    <row r="17" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>157</v>
       </c>
@@ -2786,7 +2838,7 @@
       </c>
       <c r="F17" s="14"/>
     </row>
-    <row r="18" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>159</v>
       </c>
@@ -2800,9 +2852,9 @@
       </c>
       <c r="F18" s="14"/>
     </row>
-    <row r="19" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="19" t="s">
         <v>162</v>
       </c>
       <c r="C19" s="14"/>
@@ -2810,33 +2862,47 @@
       <c r="E19" s="14"/>
       <c r="F19" s="14"/>
     </row>
-    <row r="20" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
-      <c r="B20" s="14"/>
+      <c r="B20" s="14" t="s">
+        <v>164</v>
+      </c>
       <c r="C20" s="14"/>
       <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
+      <c r="E20" s="14" t="s">
+        <v>165</v>
+      </c>
       <c r="F20" s="14"/>
     </row>
-    <row r="21" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
-      <c r="B21" s="14"/>
+      <c r="B21" s="14" t="s">
+        <v>166</v>
+      </c>
       <c r="C21" s="14"/>
       <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
+      <c r="E21" s="14" t="s">
+        <v>167</v>
+      </c>
       <c r="F21" s="14"/>
     </row>
-    <row r="22" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
-      <c r="B22" s="14"/>
+      <c r="B22" s="14" t="s">
+        <v>168</v>
+      </c>
       <c r="C22" s="14"/>
       <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
+      <c r="E22" s="14" t="s">
+        <v>169</v>
+      </c>
       <c r="F22" s="14"/>
     </row>
-    <row r="23" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
-      <c r="B23" s="14"/>
+      <c r="B23" s="14" t="s">
+        <v>170</v>
+      </c>
       <c r="C23" s="14"/>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>

</xml_diff>

<commit_message>
Gremling query language small evaluation
</commit_message>
<xml_diff>
--- a/papers/references.xlsx
+++ b/papers/references.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ansk\github\Master-s-thesis\papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF2792A-53A4-4891-A9C0-29186FAFB6DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ECBCA00-769C-4EAE-A2EF-72BD76A72BC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model-driven engineering" sheetId="1" r:id="rId1"/>
@@ -1059,11 +1059,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1933,17 +1933,17 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" customWidth="1"/>
+    <col min="2" max="2" width="26.5546875" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="64.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="64.44140625" customWidth="1"/>
     <col min="6" max="6" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1963,7 +1963,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -1983,7 +1983,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -2003,7 +2003,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>6</v>
       </c>
@@ -2023,7 +2023,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -2043,7 +2043,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
@@ -2063,7 +2063,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="225" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>19</v>
       </c>
@@ -2100,17 +2100,17 @@
       <selection activeCell="F1" sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="67.7109375" customWidth="1"/>
-    <col min="6" max="6" width="27.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="67.6640625" customWidth="1"/>
+    <col min="6" max="6" width="27.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2130,7 +2130,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>50</v>
       </c>
@@ -2145,13 +2145,13 @@
       <c r="F2" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-    </row>
-    <row r="3" spans="1:10" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+    </row>
+    <row r="3" spans="1:10" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>41</v>
       </c>
@@ -2168,11 +2168,11 @@
       <c r="F3" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-    </row>
-    <row r="4" spans="1:10" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+    </row>
+    <row r="4" spans="1:10" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>62</v>
       </c>
@@ -2186,7 +2186,7 @@
       </c>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:10" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>58</v>
       </c>
@@ -2202,7 +2202,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="390" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>43</v>
       </c>
@@ -2222,7 +2222,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="360" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>64</v>
       </c>
@@ -2255,42 +2255,42 @@
       <selection activeCell="A7" sqref="A7:F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="66.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.5546875" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" customWidth="1"/>
+    <col min="5" max="5" width="66.6640625" customWidth="1"/>
     <col min="6" max="6" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -2310,7 +2310,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>76</v>
       </c>
@@ -2326,7 +2326,7 @@
       </c>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>77</v>
       </c>
@@ -2338,7 +2338,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>78</v>
       </c>
@@ -2352,7 +2352,7 @@
       </c>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>79</v>
       </c>
@@ -2380,17 +2380,17 @@
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="5" max="5" width="71.85546875" customWidth="1"/>
-    <col min="6" max="6" width="36.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="5" max="5" width="71.88671875" customWidth="1"/>
+    <col min="6" max="6" width="36.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2410,7 +2410,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>84</v>
       </c>
@@ -2424,7 +2424,7 @@
       </c>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>87</v>
       </c>
@@ -2438,7 +2438,7 @@
       </c>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>89</v>
       </c>
@@ -2452,7 +2452,7 @@
       </c>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>91</v>
       </c>
@@ -2466,7 +2466,7 @@
       </c>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>93</v>
       </c>
@@ -2480,7 +2480,7 @@
       </c>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -2488,7 +2488,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -2496,7 +2496,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -2516,22 +2516,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{909D06DD-0136-4BF5-A323-796F63E6F11F}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="42.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" customWidth="1"/>
-    <col min="5" max="5" width="80.85546875" customWidth="1"/>
-    <col min="6" max="6" width="33.140625" customWidth="1"/>
-    <col min="8" max="8" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.109375" customWidth="1"/>
+    <col min="5" max="5" width="80.88671875" customWidth="1"/>
+    <col min="6" max="6" width="33.109375" customWidth="1"/>
+    <col min="8" max="8" width="150.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2551,7 +2551,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>122</v>
       </c>
@@ -2572,7 +2572,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>118</v>
       </c>
@@ -2595,7 +2595,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>116</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>115</v>
       </c>
@@ -2641,7 +2641,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>110</v>
       </c>
@@ -2661,7 +2661,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>109</v>
       </c>
@@ -2682,7 +2682,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>114</v>
       </c>
@@ -2705,7 +2705,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>117</v>
       </c>
@@ -2723,7 +2723,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>112</v>
       </c>
@@ -2741,7 +2741,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
         <v>111</v>
       </c>
@@ -2756,11 +2756,11 @@
       <c r="F11" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="H11" s="19" t="s">
+      <c r="H11" s="18" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>113</v>
       </c>
@@ -2776,9 +2776,9 @@
         <v>141</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="18" t="s">
         <v>148</v>
       </c>
       <c r="C13" s="14"/>
@@ -2786,7 +2786,7 @@
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
     </row>
-    <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
         <v>149</v>
       </c>
@@ -2800,7 +2800,7 @@
       </c>
       <c r="F14" s="14"/>
     </row>
-    <row r="15" spans="1:8" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
         <v>153</v>
       </c>
@@ -2812,7 +2812,7 @@
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
     </row>
-    <row r="16" spans="1:8" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
         <v>154</v>
       </c>
@@ -2824,7 +2824,7 @@
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
     </row>
-    <row r="17" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
         <v>157</v>
       </c>
@@ -2838,7 +2838,7 @@
       </c>
       <c r="F17" s="14"/>
     </row>
-    <row r="18" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="s">
         <v>159</v>
       </c>
@@ -2852,9 +2852,9 @@
       </c>
       <c r="F18" s="14"/>
     </row>
-    <row r="19" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="18" t="s">
         <v>162</v>
       </c>
       <c r="C19" s="14"/>
@@ -2862,7 +2862,7 @@
       <c r="E19" s="14"/>
       <c r="F19" s="14"/>
     </row>
-    <row r="20" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="14"/>
       <c r="B20" s="14" t="s">
         <v>164</v>
@@ -2874,7 +2874,7 @@
       </c>
       <c r="F20" s="14"/>
     </row>
-    <row r="21" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="B21" s="14" t="s">
         <v>166</v>
@@ -2886,7 +2886,7 @@
       </c>
       <c r="F21" s="14"/>
     </row>
-    <row r="22" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
       <c r="B22" s="14" t="s">
         <v>168</v>
@@ -2898,7 +2898,7 @@
       </c>
       <c r="F22" s="14"/>
     </row>
-    <row r="23" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="14"/>
       <c r="B23" s="14" t="s">
         <v>170</v>

</xml_diff>

<commit_message>
Still introduction, MCA concept is interesting for potential consideration in the future
</commit_message>
<xml_diff>
--- a/papers/references.xlsx
+++ b/papers/references.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ansk\github\Master-s-thesis\papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5087C106-5547-4385-BF49-92E33D722590}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF0700B0-DC12-46B0-AFAA-A37AD45A430E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model-driven engineering" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="174">
   <si>
     <t>Citation</t>
   </si>
@@ -870,12 +870,30 @@
   <si>
     <t>KalNdoquery: A Visual Query Language for Object Databases</t>
   </si>
+  <si>
+    <t>"@article{blair2009models,
+  title={Models@ run. time},
+  author={Blair, Gordon and Bencomo, Nelly and France, Robert B},
+  journal={Computer},
+  volume={42},
+  number={10},
+  pages={22--27},
+  year={2009},
+  publisher={IEEE}
+}"</t>
+  </si>
+  <si>
+    <t>Models@Runt.time</t>
+  </si>
+  <si>
+    <t>Perfect paper with many basic concepts. Use it as a bridge in your introduction to considering models during runtime after reasoning about the power of model in software development</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -898,6 +916,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1005,10 +1031,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1065,8 +1092,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="49">
@@ -2376,8 +2407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C75DB7F1-B501-46CE-AB52-85AC9D327FEE}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2481,12 +2512,18 @@
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
+      <c r="A7" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>172</v>
+      </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
+      <c r="F7" s="5" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
@@ -2505,9 +2542,12 @@
       <c r="F9" s="5"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{481AA373-8799-47C8-8D23-03B1372C0A4C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2516,7 +2556,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{909D06DD-0136-4BF5-A323-796F63E6F11F}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixes in introduction. Writing the foundation chapter
</commit_message>
<xml_diff>
--- a/papers/references.xlsx
+++ b/papers/references.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ansk\github\Master-s-thesis\papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF0700B0-DC12-46B0-AFAA-A37AD45A430E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1921C8E2-2A16-4875-8CAF-23486EE78710}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model-driven engineering" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="175">
   <si>
     <t>Citation</t>
   </si>
@@ -335,9 +335,6 @@
     <t xml:space="preserve">Using either UML profiles or metamodels, one can define a custom DSL. Two necessary parts of DSL are semantics and syntax. One can either use UML while stereotypes or tagged values for DSL. Alternatively, one can utilize the M3 level to define the DSL metamodel.
 On the one hand, UML is a rich tool with a lot of functionality. However, its known limitation, as stated here, is that it lacks the semantics used by domain experts and is limited when describing technical domain concepts.
 </t>
-  </si>
-  <si>
-    <t>A metamodel hierarchy is shown in Figure 1. On its top level is a meta-meta model or a graph schema of a language. This level hosts concepts and rules for the level below. The concept that might be difficult to grasp at first glance is that the M3 level is self-descriptive. Many M3 languages can be used to describe themselves on the M2 level. The property of being self-descriptive or lifted as stated here [] is the reason why there is no more level in a classical metamodeling hierarchy. M2 level contains language specifications. For example, UML concepts are defined at this level. Level M1 has software classes or application concepts. The M0 level contains real objects that are instances of the M1 level. Also, there is the M-1 level which is a real-world where software objects have digital twins of real objects. Digital twin takes the state of a real object at runtime.</t>
   </si>
   <si>
     <t>Answer the following questions:</t>
@@ -887,6 +884,12 @@
   </si>
   <si>
     <t>Perfect paper with many basic concepts. Use it as a bridge in your introduction to considering models during runtime after reasoning about the power of model in software development</t>
+  </si>
+  <si>
+    <t>"@ARTICLE{1231149,  author={Atkinson, C. and Kuhne, T.},  journal={IEEE Software},   title={Model-driven development: a metamodeling foundation},   year={2003},  volume={20},  number={5},  pages={36-41},  doi={10.1109/MS.2003.1231149}}"</t>
+  </si>
+  <si>
+    <t>Explained metamodeling hierarchy</t>
   </si>
 </sst>
 </file>
@@ -1089,11 +1092,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1633,8 +1636,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{822ADA59-34C7-4394-AE31-5D8AD6802D70}" name="Table3" displayName="Table3" ref="A1:F7" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36">
-  <autoFilter ref="A1:F7" xr:uid="{DBC3082E-8AB2-4060-B752-8823303D327C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{822ADA59-34C7-4394-AE31-5D8AD6802D70}" name="Table3" displayName="Table3" ref="A1:F8" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36">
+  <autoFilter ref="A1:F8" xr:uid="{DBC3082E-8AB2-4060-B752-8823303D327C}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{04A3358C-38AC-41A2-9EF8-F78CF5E86A8B}" name="Citation" dataDxfId="34"/>
     <tableColumn id="2" xr3:uid="{07437842-31FC-44BC-A480-C79738F8C3E8}" name="Paper" dataDxfId="33"/>
@@ -2125,10 +2128,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CF1A488-2851-4C66-A331-30E6C95E0D1D}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F1" sqref="A1:F1"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2176,11 +2179,9 @@
       <c r="F2" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="H2" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
     </row>
     <row r="3" spans="1:10" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
@@ -2199,9 +2200,9 @@
       <c r="F3" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
     </row>
     <row r="4" spans="1:10" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
@@ -2266,14 +2267,29 @@
         <v>65</v>
       </c>
       <c r="F7" s="12"/>
+    </row>
+    <row r="8" spans="1:10" ht="273.60000000000002" x14ac:dyDescent="0.3">
+      <c r="A8" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12" t="s">
+        <v>174</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="H2:J3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2298,27 +2314,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -2343,26 +2359,26 @@
     </row>
     <row r="8" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F8" s="6"/>
     </row>
     <row r="9" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -2371,24 +2387,24 @@
     </row>
     <row r="10" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -2407,7 +2423,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C75DB7F1-B501-46CE-AB52-85AC9D327FEE}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -2443,86 +2459,86 @@
     </row>
     <row r="2" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B7" s="19" t="s">
         <v>171</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>172</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2556,7 +2572,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{909D06DD-0136-4BF5-A323-796F63E6F11F}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -2579,7 +2595,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>12</v>
@@ -2593,200 +2609,200 @@
     </row>
     <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>122</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>123</v>
       </c>
       <c r="C2" s="14">
         <v>1437</v>
       </c>
       <c r="D2" s="14"/>
       <c r="E2" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C3" s="14">
         <v>20</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E3" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="F3" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="F3" s="14" t="s">
-        <v>146</v>
-      </c>
       <c r="H3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C4" s="14">
         <v>47</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C5" s="14">
         <v>60</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E5" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="F5" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="F5" s="14" t="s">
-        <v>139</v>
-      </c>
       <c r="H5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C6" s="14">
         <v>98</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C7" s="14">
         <v>79</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C8" s="14">
         <v>229</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E8" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="F8" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="F8" s="14" t="s">
-        <v>120</v>
-      </c>
       <c r="H8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C9" s="14">
         <v>153</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C10" s="14">
         <v>109</v>
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C11" s="15">
         <v>168</v>
@@ -2794,18 +2810,18 @@
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
       <c r="F11" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H11" s="18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C12" s="15">
         <v>131</v>
@@ -2813,13 +2829,13 @@
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
       <c r="F12" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
       <c r="B13" s="18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
@@ -2828,24 +2844,24 @@
     </row>
     <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="B14" s="14" t="s">
         <v>149</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>150</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="14"/>
       <c r="E14" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F14" s="14"/>
     </row>
     <row r="15" spans="1:8" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
@@ -2854,10 +2870,10 @@
     </row>
     <row r="16" spans="1:8" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="B16" s="15" t="s">
         <v>154</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>155</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
@@ -2866,36 +2882,36 @@
     </row>
     <row r="17" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="14"/>
       <c r="E17" s="14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F17" s="14"/>
     </row>
     <row r="18" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C18" s="14"/>
       <c r="D18" s="14"/>
       <c r="E18" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F18" s="14"/>
     </row>
     <row r="19" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
       <c r="B19" s="18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C19" s="14"/>
       <c r="D19" s="14"/>
@@ -2905,43 +2921,43 @@
     <row r="20" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="14"/>
       <c r="B20" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C20" s="14"/>
       <c r="D20" s="14"/>
       <c r="E20" s="14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F20" s="14"/>
     </row>
     <row r="21" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="B21" s="14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C21" s="14"/>
       <c r="D21" s="14"/>
       <c r="E21" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F21" s="14"/>
     </row>
     <row r="22" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
       <c r="B22" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C22" s="14"/>
       <c r="D22" s="14"/>
       <c r="E22" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F22" s="14"/>
     </row>
     <row r="23" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="14"/>
       <c r="B23" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C23" s="14"/>
       <c r="D23" s="14"/>

</xml_diff>

<commit_message>
Foundation chapter is ready (subchapter about variant-aware models is left for later)
</commit_message>
<xml_diff>
--- a/papers/references.xlsx
+++ b/papers/references.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ansk\github\Master-s-thesis\papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1921C8E2-2A16-4875-8CAF-23486EE78710}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41A0C2E-07FF-4437-90E6-BFF965231CFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="16470" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model-driven engineering" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="179">
   <si>
     <t>Citation</t>
   </si>
@@ -748,9 +748,6 @@
     <t xml:space="preserve">Predefined queries (PDQ) -&gt; to predefined constraints?? </t>
   </si>
   <si>
-    <t>Both of these disadvantages are avoided by Constraint Diagrams [4]. Here, the concrete syntax (which is much less likely to change than the meta-model) is used to formulate a query. Unfortunately, Constraint Diagrams are rather limited with respect to the modeling language they may be applied to (basic class diagrams). Also, it seems that Constraint Diagrams have never been implemented as a tool.</t>
-  </si>
-  <si>
     <t>User-driven query system for modelling mde artifacts</t>
   </si>
   <si>
@@ -890,6 +887,27 @@
   </si>
   <si>
     <t>Explained metamodeling hierarchy</t>
+  </si>
+  <si>
+    <t>"@INPROCEEDINGS{989813,  author={Bezivin, J. and Gerbe, O.},  booktitle={Proceedings 16th Annual International Conference on Automated Software Engineering (ASE 2001)},   title={Towards a precise definition of the OMG/MDA framework},   year={2001},  volume={},  number={},  pages={273-280},  doi={10.1109/ASE.2001.989813}}"</t>
+  </si>
+  <si>
+    <t>Towards a precise definition of the OMG/MDA framework</t>
+  </si>
+  <si>
+    <t>Both of these disadvantages are avo ided by Constraint Diagrams [4]. Here, the concrete syntax (which is much less likely to change than the meta-model) is used to formulate a query. Unfortunately, Constraint Diagrams are rather limited with respect to the modeling language they may be applied to (basic class diagrams). Also, it seems that Constraint Diagrams have never been implemented as a tool.</t>
+  </si>
+  <si>
+    <t>Another major difference between multi-level modeling environments and traditional modeling technologies is that one can change all levels of a multi-level
+model at the same time. Changes on one level immediately effect all other levels. We usually refer to this concept as real-time (meta-)modeling. In traditional
+meta-modeling environments the meta-model is fixed when editing a meta-model instance (i.e. a model). Moreover, when editing a meta-model, instances of that
+model are usually not directly accessible. Because only two levels are ever available for modeling (usually the meta-model and model), we refer to such environments as two-level modeling environments. The limitations of such environments
+make it difficult for a language engineer to alter more than one level on-the-fly
+during model creation. When all model levels are equally available for modeling
+at all times new possibilities for creating, debugging and extending domainspecific modeling languages are created.</t>
+  </si>
+  <si>
+    <t>focuses on the preservance of integraty constraint validity during the development of design concepts.</t>
   </si>
 </sst>
 </file>
@@ -1076,9 +1094,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1093,6 +1108,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1636,8 +1654,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{822ADA59-34C7-4394-AE31-5D8AD6802D70}" name="Table3" displayName="Table3" ref="A1:F8" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36">
-  <autoFilter ref="A1:F8" xr:uid="{DBC3082E-8AB2-4060-B752-8823303D327C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{822ADA59-34C7-4394-AE31-5D8AD6802D70}" name="Table3" displayName="Table3" ref="A1:F10" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36">
+  <autoFilter ref="A1:F10" xr:uid="{DBC3082E-8AB2-4060-B752-8823303D327C}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{04A3358C-38AC-41A2-9EF8-F78CF5E86A8B}" name="Citation" dataDxfId="34"/>
     <tableColumn id="2" xr3:uid="{07437842-31FC-44BC-A480-C79738F8C3E8}" name="Paper" dataDxfId="33"/>
@@ -1963,21 +1981,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" customWidth="1"/>
-    <col min="2" max="2" width="26.5546875" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
-    <col min="5" max="5" width="64.44140625" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="64.42578125" customWidth="1"/>
     <col min="6" max="6" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1997,7 +2015,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -2017,7 +2035,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -2037,7 +2055,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>6</v>
       </c>
@@ -2057,7 +2075,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -2077,7 +2095,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
@@ -2097,7 +2115,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="225" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>19</v>
       </c>
@@ -2128,23 +2146,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CF1A488-2851-4C66-A331-30E6C95E0D1D}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" customWidth="1"/>
-    <col min="5" max="5" width="67.6640625" customWidth="1"/>
-    <col min="6" max="6" width="27.5546875" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="67.7109375" customWidth="1"/>
+    <col min="6" max="6" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2164,7 +2182,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>50</v>
       </c>
@@ -2183,7 +2201,7 @@
       <c r="I2" s="20"/>
       <c r="J2" s="20"/>
     </row>
-    <row r="3" spans="1:10" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>41</v>
       </c>
@@ -2204,7 +2222,7 @@
       <c r="I3" s="20"/>
       <c r="J3" s="20"/>
     </row>
-    <row r="4" spans="1:10" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>62</v>
       </c>
@@ -2218,7 +2236,7 @@
       </c>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:10" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>58</v>
       </c>
@@ -2234,7 +2252,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="331.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="390" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>43</v>
       </c>
@@ -2254,7 +2272,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="331.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="360" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>64</v>
       </c>
@@ -2268,19 +2286,39 @@
       </c>
       <c r="F7" s="12"/>
     </row>
-    <row r="8" spans="1:10" ht="273.60000000000002" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>8</v>
-      </c>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="12"/>
+    </row>
+    <row r="9" spans="1:10" ht="300" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="405" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
         <v>174</v>
       </c>
+      <c r="B10" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2298,46 +2336,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{171206E4-2EA6-4B1F-83FB-DEC77FFB9355}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:F7"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5546875" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" customWidth="1"/>
-    <col min="5" max="5" width="66.6640625" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="66.7109375" customWidth="1"/>
     <col min="6" max="6" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -2357,7 +2395,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>75</v>
       </c>
@@ -2373,7 +2411,7 @@
       </c>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>76</v>
       </c>
@@ -2385,7 +2423,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>77</v>
       </c>
@@ -2399,7 +2437,7 @@
       </c>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>78</v>
       </c>
@@ -2423,21 +2461,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C75DB7F1-B501-46CE-AB52-85AC9D327FEE}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" customWidth="1"/>
-    <col min="5" max="5" width="71.88671875" customWidth="1"/>
-    <col min="6" max="6" width="36.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="71.85546875" customWidth="1"/>
+    <col min="6" max="6" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2457,7 +2495,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>83</v>
       </c>
@@ -2471,7 +2509,7 @@
       </c>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>86</v>
       </c>
@@ -2485,11 +2523,11 @@
       </c>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="19" t="s">
         <v>87</v>
       </c>
       <c r="C4" s="5"/>
@@ -2499,7 +2537,7 @@
       </c>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>90</v>
       </c>
@@ -2513,7 +2551,7 @@
       </c>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>92</v>
       </c>
@@ -2527,21 +2565,21 @@
       </c>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="B7" s="18" t="s">
         <v>170</v>
-      </c>
-      <c r="B7" s="19" t="s">
-        <v>171</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -2549,7 +2587,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -2560,34 +2598,35 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{481AA373-8799-47C8-8D23-03B1372C0A4C}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{7BFE404F-6122-4536-87AB-7A72CF5A8042}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{909D06DD-0136-4BF5-A323-796F63E6F11F}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="2" max="2" width="42.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.109375" customWidth="1"/>
-    <col min="5" max="5" width="80.88671875" customWidth="1"/>
-    <col min="6" max="6" width="33.109375" customWidth="1"/>
-    <col min="8" max="8" width="150.6640625" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" customWidth="1"/>
+    <col min="5" max="5" width="80.85546875" customWidth="1"/>
+    <col min="6" max="6" width="33.140625" customWidth="1"/>
+    <col min="8" max="8" width="150.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2607,7 +2646,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>121</v>
       </c>
@@ -2624,11 +2663,11 @@
       <c r="F2" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="15" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>117</v>
       </c>
@@ -2642,16 +2681,16 @@
         <v>133</v>
       </c>
       <c r="E3" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="F3" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="F3" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="H3" s="15" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>115</v>
       </c>
@@ -2670,11 +2709,11 @@
       <c r="F4" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="15" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>114</v>
       </c>
@@ -2693,31 +2732,31 @@
       <c r="F5" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="15" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
+    <row r="6" spans="1:8" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="13">
         <v>98</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="13" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>108</v>
       </c>
@@ -2734,11 +2773,11 @@
       <c r="F7" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="15" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>113</v>
       </c>
@@ -2757,212 +2796,222 @@
       <c r="F8" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="15" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="14" t="s">
+    <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="13">
         <v>153</v>
       </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14" t="s">
+      <c r="D9" s="13"/>
+      <c r="E9" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="13" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="14" t="s">
+    <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="13">
         <v>109</v>
       </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14" t="s">
+      <c r="D10" s="13"/>
+      <c r="E10" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="13" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C11" s="14">
+        <v>168</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="C12" s="14">
+        <v>131</v>
+      </c>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="16" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="13"/>
+      <c r="B13" s="17" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="C11" s="15">
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+    </row>
+    <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="F14" s="13"/>
+    </row>
+    <row r="15" spans="1:8" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+    </row>
+    <row r="16" spans="1:8" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+    </row>
+    <row r="17" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="C17" s="14"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="F17" s="13"/>
+    </row>
+    <row r="18" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="F18" s="13"/>
+    </row>
+    <row r="19" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
+      <c r="B19" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+    </row>
+    <row r="20" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
+      <c r="B20" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="F20" s="13"/>
+    </row>
+    <row r="21" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="13"/>
+      <c r="B21" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="F21" s="13"/>
+    </row>
+    <row r="22" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="13"/>
+      <c r="B22" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="F22" s="13"/>
+    </row>
+    <row r="23" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="13"/>
+      <c r="B23" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="H11" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="C12" s="15">
-        <v>131</v>
-      </c>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="17" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="14"/>
-      <c r="B13" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-    </row>
-    <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="F14" s="14"/>
-    </row>
-    <row r="15" spans="1:8" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-    </row>
-    <row r="16" spans="1:8" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-    </row>
-    <row r="17" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="F17" s="14"/>
-    </row>
-    <row r="18" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="F18" s="14"/>
-    </row>
-    <row r="19" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="14"/>
-      <c r="B19" s="18" t="s">
-        <v>161</v>
-      </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-    </row>
-    <row r="20" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="14"/>
-      <c r="B20" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="F20" s="14"/>
-    </row>
-    <row r="21" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="14"/>
-      <c r="B21" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14" t="s">
-        <v>166</v>
-      </c>
-      <c r="F21" s="14"/>
-    </row>
-    <row r="22" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="14"/>
-      <c r="B22" s="14" t="s">
-        <v>167</v>
-      </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="F22" s="14"/>
-    </row>
-    <row r="23" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="14"/>
-      <c r="B23" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="195" x14ac:dyDescent="0.25">
+      <c r="E27" s="17" t="s">
+        <v>177</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Concept and requirements chapter is ready
</commit_message>
<xml_diff>
--- a/papers/references.xlsx
+++ b/papers/references.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ansk\github\Master-s-thesis\papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41A0C2E-07FF-4437-90E6-BFF965231CFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{757AE401-B81D-44A5-A8D1-FC06076AE09F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="16470" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model-driven engineering" sheetId="1" r:id="rId1"/>
@@ -1985,17 +1985,17 @@
       <selection activeCell="A2" sqref="A2:F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" customWidth="1"/>
+    <col min="2" max="2" width="26.5546875" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="64.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="64.44140625" customWidth="1"/>
     <col min="6" max="6" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2015,7 +2015,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -2055,7 +2055,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>6</v>
       </c>
@@ -2075,7 +2075,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -2095,7 +2095,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
@@ -2115,7 +2115,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="225" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>19</v>
       </c>
@@ -2152,17 +2152,17 @@
       <selection activeCell="A2" sqref="A2:F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="67.7109375" customWidth="1"/>
-    <col min="6" max="6" width="27.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="67.6640625" customWidth="1"/>
+    <col min="6" max="6" width="27.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2182,7 +2182,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>50</v>
       </c>
@@ -2201,7 +2201,7 @@
       <c r="I2" s="20"/>
       <c r="J2" s="20"/>
     </row>
-    <row r="3" spans="1:10" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>41</v>
       </c>
@@ -2222,7 +2222,7 @@
       <c r="I3" s="20"/>
       <c r="J3" s="20"/>
     </row>
-    <row r="4" spans="1:10" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>62</v>
       </c>
@@ -2236,7 +2236,7 @@
       </c>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:10" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>58</v>
       </c>
@@ -2252,7 +2252,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="390" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>43</v>
       </c>
@@ -2272,7 +2272,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="360" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>64</v>
       </c>
@@ -2286,7 +2286,7 @@
       </c>
       <c r="F7" s="12"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
@@ -2294,7 +2294,7 @@
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
     </row>
-    <row r="9" spans="1:10" ht="300" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>172</v>
       </c>
@@ -2308,7 +2308,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="405" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="374.4" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>174</v>
       </c>
@@ -2340,42 +2340,42 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="66.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.5546875" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" customWidth="1"/>
+    <col min="5" max="5" width="66.6640625" customWidth="1"/>
     <col min="6" max="6" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -2395,7 +2395,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>75</v>
       </c>
@@ -2411,7 +2411,7 @@
       </c>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>76</v>
       </c>
@@ -2423,7 +2423,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>77</v>
       </c>
@@ -2437,7 +2437,7 @@
       </c>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>78</v>
       </c>
@@ -2465,17 +2465,17 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="5" max="5" width="71.85546875" customWidth="1"/>
-    <col min="6" max="6" width="36.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="5" max="5" width="71.88671875" customWidth="1"/>
+    <col min="6" max="6" width="36.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2495,7 +2495,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>83</v>
       </c>
@@ -2509,7 +2509,7 @@
       </c>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>86</v>
       </c>
@@ -2523,7 +2523,7 @@
       </c>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>88</v>
       </c>
@@ -2537,7 +2537,7 @@
       </c>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>90</v>
       </c>
@@ -2551,7 +2551,7 @@
       </c>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>92</v>
       </c>
@@ -2565,7 +2565,7 @@
       </c>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>169</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -2587,7 +2587,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -2611,22 +2611,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{909D06DD-0136-4BF5-A323-796F63E6F11F}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="42.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" customWidth="1"/>
-    <col min="5" max="5" width="80.85546875" customWidth="1"/>
-    <col min="6" max="6" width="33.140625" customWidth="1"/>
-    <col min="8" max="8" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.109375" customWidth="1"/>
+    <col min="5" max="5" width="80.88671875" customWidth="1"/>
+    <col min="6" max="6" width="33.109375" customWidth="1"/>
+    <col min="8" max="8" width="150.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2646,7 +2646,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>121</v>
       </c>
@@ -2667,7 +2667,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>117</v>
       </c>
@@ -2690,7 +2690,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>115</v>
       </c>
@@ -2713,7 +2713,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>114</v>
       </c>
@@ -2736,7 +2736,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>109</v>
       </c>
@@ -2756,7 +2756,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>108</v>
       </c>
@@ -2777,7 +2777,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>113</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>116</v>
       </c>
@@ -2818,7 +2818,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>111</v>
       </c>
@@ -2836,7 +2836,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>110</v>
       </c>
@@ -2855,7 +2855,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
         <v>112</v>
       </c>
@@ -2871,7 +2871,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13"/>
       <c r="B13" s="17" t="s">
         <v>146</v>
@@ -2881,7 +2881,7 @@
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
     </row>
-    <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
         <v>147</v>
       </c>
@@ -2895,7 +2895,7 @@
       </c>
       <c r="F14" s="13"/>
     </row>
-    <row r="15" spans="1:8" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
         <v>151</v>
       </c>
@@ -2907,7 +2907,7 @@
       <c r="E15" s="14"/>
       <c r="F15" s="14"/>
     </row>
-    <row r="16" spans="1:8" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>152</v>
       </c>
@@ -2919,7 +2919,7 @@
       <c r="E16" s="14"/>
       <c r="F16" s="14"/>
     </row>
-    <row r="17" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
         <v>155</v>
       </c>
@@ -2933,7 +2933,7 @@
       </c>
       <c r="F17" s="13"/>
     </row>
-    <row r="18" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
         <v>157</v>
       </c>
@@ -2947,7 +2947,7 @@
       </c>
       <c r="F18" s="13"/>
     </row>
-    <row r="19" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13"/>
       <c r="B19" s="17" t="s">
         <v>160</v>
@@ -2957,7 +2957,7 @@
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
     </row>
-    <row r="20" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13"/>
       <c r="B20" s="13" t="s">
         <v>162</v>
@@ -2969,7 +2969,7 @@
       </c>
       <c r="F20" s="13"/>
     </row>
-    <row r="21" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="13"/>
       <c r="B21" s="13" t="s">
         <v>164</v>
@@ -2981,7 +2981,7 @@
       </c>
       <c r="F21" s="13"/>
     </row>
-    <row r="22" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="13"/>
       <c r="B22" s="13" t="s">
         <v>166</v>
@@ -2993,7 +2993,7 @@
       </c>
       <c r="F22" s="13"/>
     </row>
-    <row r="23" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="13"/>
       <c r="B23" s="13" t="s">
         <v>168</v>
@@ -3003,12 +3003,12 @@
       <c r="E23" s="13"/>
       <c r="F23" s="13"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="195" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="187.2" x14ac:dyDescent="0.3">
       <c r="E27" s="17" t="s">
         <v>177</v>
       </c>

</xml_diff>